<commit_message>
general and switch tabs
</commit_message>
<xml_diff>
--- a/CPYDAR/ieee13x.xlsx
+++ b/CPYDAR/ieee13x.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="General" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Switch" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,67 +435,188 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="n">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Excel file version</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>v2.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>ieee13pv</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Frequency (Hz)</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Power Base (MVA)</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>From Bus</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>To Bus</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>650</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>brkr</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>brkr1</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Excel file version</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>v2.0</t>
-        </is>
-      </c>
-    </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>633</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>xf1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>fuse1</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>ieee13x</t>
-        </is>
-      </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>671</t>
+        </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Frequency (Hz)</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>60</v>
+          <t>692</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>671692</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>684</t>
+        </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Power Base (MVA)</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>100</v>
+          <t>tap</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>sect1</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>632</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>mid</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>rec1</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
voltage source and bus sheets
</commit_message>
<xml_diff>
--- a/CPYDAR/ieee13x.xlsx
+++ b/CPYDAR/ieee13x.xlsx
@@ -8,7 +8,9 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="General" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Switch" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Voltage Source" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Bus" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Switch" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -489,6 +491,680 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A13:F14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B13" s="1" t="inlineStr">
+        <is>
+          <t>Bus</t>
+        </is>
+      </c>
+      <c r="C13" s="1" t="inlineStr">
+        <is>
+          <t>Voltage (pu)</t>
+        </is>
+      </c>
+      <c r="D13" s="1" t="inlineStr">
+        <is>
+          <t>Angle (deg)</t>
+        </is>
+      </c>
+      <c r="E13" s="1" t="inlineStr">
+        <is>
+          <t>Rs (pu)</t>
+        </is>
+      </c>
+      <c r="F13" s="1" t="inlineStr">
+        <is>
+          <t>Xs (pu)</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>sourcebus</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>115000</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>source</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>0.001212678109640832</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.001212678109640832</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Bus</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Base Voltage (V)</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Initial Vmag</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Unit (V, pu)</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Angle (deg)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>611</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>4160</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>PQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>632</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>4160</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>PQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>633</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>4160</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>PQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>634</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>480</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>PV</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>645</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>4160</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>PQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>646</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>4160</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>PQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>650</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>4160</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>PQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>652</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>4160</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>PQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>670</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>4160</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>PQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>671</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>4160</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>PQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>675</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>4160</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>PQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>680</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>4160</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>PQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>684</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>4160</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>PQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>692</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>4160</v>
+      </c>
+      <c r="C15" t="n">
+        <v>1</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>PQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>brkr</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>4160</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>PQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>house</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>208</v>
+      </c>
+      <c r="C17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>PV</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>mid</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>4160</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>PQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>rg60</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>4160</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>PQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>sourcebus</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>115000</v>
+      </c>
+      <c r="C20" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>SLACK</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>tap</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>4160</v>
+      </c>
+      <c r="C21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>PQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>xf1</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>4160</v>
+      </c>
+      <c r="C22" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>PQ</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
handles phasing for bus, voltage source, switch
</commit_message>
<xml_diff>
--- a/CPYDAR/ieee13x.xlsx
+++ b/CPYDAR/ieee13x.xlsx
@@ -491,7 +491,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A13:F14"/>
+  <dimension ref="A11:J26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -499,62 +499,258 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Positive Sequence Voltage Source</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B12" s="1" t="inlineStr">
+        <is>
+          <t>Bus</t>
+        </is>
+      </c>
+      <c r="C12" s="1" t="inlineStr">
+        <is>
+          <t>Voltage (pu)</t>
+        </is>
+      </c>
+      <c r="D12" s="1" t="inlineStr">
+        <is>
+          <t>Angle (deg)</t>
+        </is>
+      </c>
+      <c r="E12" s="1" t="inlineStr">
+        <is>
+          <t>Rs (pu)</t>
+        </is>
+      </c>
+      <c r="F12" s="1" t="inlineStr">
+        <is>
+          <t>Xs (pu)</t>
+        </is>
+      </c>
+    </row>
     <row r="13">
-      <c r="A13" s="1" t="inlineStr">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>End of Positive Sequence Voltage Source</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Single-Phase Voltage Source</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="B13" s="1" t="inlineStr">
-        <is>
-          <t>Bus</t>
-        </is>
-      </c>
-      <c r="C13" s="1" t="inlineStr">
-        <is>
-          <t>Voltage (pu)</t>
-        </is>
-      </c>
-      <c r="D13" s="1" t="inlineStr">
+      <c r="B16" s="1" t="inlineStr">
+        <is>
+          <t>Bus1</t>
+        </is>
+      </c>
+      <c r="C16" s="1" t="inlineStr">
+        <is>
+          <t>Voltage (V)</t>
+        </is>
+      </c>
+      <c r="D16" s="1" t="inlineStr">
         <is>
           <t>Angle (deg)</t>
         </is>
       </c>
-      <c r="E13" s="1" t="inlineStr">
-        <is>
-          <t>Rs (pu)</t>
-        </is>
-      </c>
-      <c r="F13" s="1" t="inlineStr">
-        <is>
-          <t>Xs (pu)</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="E16" s="1" t="inlineStr">
+        <is>
+          <t>Rs (Ohm)</t>
+        </is>
+      </c>
+      <c r="F16" s="1" t="inlineStr">
+        <is>
+          <t>Xs (Ohm)</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>End of Single-Phase Voltage Source</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Three-Phase Voltage Source with Short-Circuit Level Data</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B20" s="1" t="inlineStr">
+        <is>
+          <t>Bus1</t>
+        </is>
+      </c>
+      <c r="C20" s="1" t="inlineStr">
+        <is>
+          <t>Bus2</t>
+        </is>
+      </c>
+      <c r="D20" s="1" t="inlineStr">
+        <is>
+          <t>Bus3</t>
+        </is>
+      </c>
+      <c r="E20" s="1" t="inlineStr">
+        <is>
+          <t>kV (ph-ph RMS)</t>
+        </is>
+      </c>
+      <c r="F20" s="1" t="inlineStr">
+        <is>
+          <t>Angle_a (deg)</t>
+        </is>
+      </c>
+      <c r="G20" s="1" t="inlineStr">
+        <is>
+          <t>SC1ph (MVA)</t>
+        </is>
+      </c>
+      <c r="H20" s="1" t="inlineStr">
+        <is>
+          <t>SC3ph (MVA)</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>End of Three-Phase Voltage Source with Short-Circuit Level Data</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Three-Phase Voltage Source with Sequential Data</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B24" s="1" t="inlineStr">
+        <is>
+          <t>Bus1</t>
+        </is>
+      </c>
+      <c r="C24" s="1" t="inlineStr">
+        <is>
+          <t>Bus2</t>
+        </is>
+      </c>
+      <c r="D24" s="1" t="inlineStr">
+        <is>
+          <t>Bus3</t>
+        </is>
+      </c>
+      <c r="E24" s="1" t="inlineStr">
+        <is>
+          <t>kV (ph-ph RMS)</t>
+        </is>
+      </c>
+      <c r="F24" s="1" t="inlineStr">
+        <is>
+          <t>Angle_a (deg)</t>
+        </is>
+      </c>
+      <c r="G24" s="1" t="inlineStr">
+        <is>
+          <t>R1 (Ohm)</t>
+        </is>
+      </c>
+      <c r="H24" s="1" t="inlineStr">
+        <is>
+          <t>X1 (Ohm)</t>
+        </is>
+      </c>
+      <c r="I24" s="1" t="inlineStr">
+        <is>
+          <t>R0 (Ohm)</t>
+        </is>
+      </c>
+      <c r="J24" s="1" t="inlineStr">
+        <is>
+          <t>X0 (Ohm)</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
         <is>
           <t>source</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>sourcebus</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>115000</v>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>source</t>
-        </is>
-      </c>
-      <c r="E14" t="n">
-        <v>0.001212678109640832</v>
-      </c>
-      <c r="F14" t="n">
-        <v>0.001212678109640832</v>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>sourcebus_A</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>sourcebus_B</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>sourcebus_C</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>115</v>
+      </c>
+      <c r="F25" t="n">
+        <v>30.0000002521989</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.16037668</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0.64150673</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0.17960358</v>
+      </c>
+      <c r="J25" t="n">
+        <v>0.53881075</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>End of Three-Phase Voltage Source with Sequential Data</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -568,7 +764,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -611,11 +807,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>611</t>
+          <t>611_C</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4160</v>
+        <v>2401.777119828843</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
@@ -626,7 +822,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -637,11 +833,11 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>632</t>
+          <t>632_B</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>4160</v>
+        <v>2401.777119828843</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
@@ -652,7 +848,7 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -663,11 +859,11 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>633</t>
+          <t>632_C</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>4160</v>
+        <v>2401.777119828843</v>
       </c>
       <c r="C4" t="n">
         <v>1</v>
@@ -678,7 +874,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -689,11 +885,11 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>634</t>
+          <t>632_A</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>480</v>
+        <v>2401.777119828843</v>
       </c>
       <c r="C5" t="n">
         <v>1</v>
@@ -708,18 +904,18 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>PV</t>
+          <t>PQ</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>645</t>
+          <t>633_B</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>4160</v>
+        <v>2401.777119828843</v>
       </c>
       <c r="C6" t="n">
         <v>1</v>
@@ -730,7 +926,7 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -741,11 +937,11 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>646</t>
+          <t>633_C</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>4160</v>
+        <v>2401.777119828843</v>
       </c>
       <c r="C7" t="n">
         <v>1</v>
@@ -756,7 +952,7 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -767,11 +963,11 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>650</t>
+          <t>633_A</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>4160</v>
+        <v>2401.777119828843</v>
       </c>
       <c r="C8" t="n">
         <v>1</v>
@@ -793,11 +989,11 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>652</t>
+          <t>634_B</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>4160</v>
+        <v>277.1281292110204</v>
       </c>
       <c r="C9" t="n">
         <v>1</v>
@@ -808,7 +1004,7 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -819,11 +1015,11 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>670</t>
+          <t>634_C</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>4160</v>
+        <v>277.1281292110204</v>
       </c>
       <c r="C10" t="n">
         <v>1</v>
@@ -834,7 +1030,7 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -845,11 +1041,11 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>671</t>
+          <t>634_A</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>4160</v>
+        <v>277.1281292110204</v>
       </c>
       <c r="C11" t="n">
         <v>1</v>
@@ -871,11 +1067,11 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>675</t>
+          <t>645_B</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>4160</v>
+        <v>2401.777119828843</v>
       </c>
       <c r="C12" t="n">
         <v>1</v>
@@ -886,7 +1082,7 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -897,11 +1093,11 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>680</t>
+          <t>645_C</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>4160</v>
+        <v>2401.777119828843</v>
       </c>
       <c r="C13" t="n">
         <v>1</v>
@@ -912,7 +1108,7 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -923,11 +1119,11 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>684</t>
+          <t>646_B</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>4160</v>
+        <v>2401.777119828843</v>
       </c>
       <c r="C14" t="n">
         <v>1</v>
@@ -938,7 +1134,7 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
@@ -949,11 +1145,11 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>692</t>
+          <t>646_C</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>4160</v>
+        <v>2401.777119828843</v>
       </c>
       <c r="C15" t="n">
         <v>1</v>
@@ -964,7 +1160,7 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -975,11 +1171,11 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>brkr</t>
+          <t>650_B</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>4160</v>
+        <v>2401.777119828843</v>
       </c>
       <c r="C16" t="n">
         <v>1</v>
@@ -990,7 +1186,7 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -1001,11 +1197,11 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>house</t>
+          <t>650_C</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>208</v>
+        <v>2401.777119828843</v>
       </c>
       <c r="C17" t="n">
         <v>1</v>
@@ -1016,22 +1212,22 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>PV</t>
+          <t>PQ</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>mid</t>
+          <t>650_A</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>4160</v>
+        <v>2401.777119828843</v>
       </c>
       <c r="C18" t="n">
         <v>1</v>
@@ -1053,11 +1249,11 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>rg60</t>
+          <t>652_A</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>4160</v>
+        <v>2401.777119828843</v>
       </c>
       <c r="C19" t="n">
         <v>1</v>
@@ -1079,11 +1275,11 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>sourcebus</t>
+          <t>670_B</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>115000</v>
+        <v>2401.777119828843</v>
       </c>
       <c r="C20" t="n">
         <v>1</v>
@@ -1094,22 +1290,22 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>SLACK</t>
+          <t>PQ</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>tap</t>
+          <t>670_C</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>4160</v>
+        <v>2401.777119828843</v>
       </c>
       <c r="C21" t="n">
         <v>1</v>
@@ -1120,7 +1316,7 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
@@ -1131,11 +1327,11 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>xf1</t>
+          <t>670_A</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>4160</v>
+        <v>2401.777119828843</v>
       </c>
       <c r="C22" t="n">
         <v>1</v>
@@ -1149,6 +1345,838 @@
         <v>0</v>
       </c>
       <c r="F22" t="inlineStr">
+        <is>
+          <t>PQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>671_B</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>2401.777119828843</v>
+      </c>
+      <c r="C23" t="n">
+        <v>1</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>-120</v>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>PQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>671_C</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>2401.777119828843</v>
+      </c>
+      <c r="C24" t="n">
+        <v>1</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>120</v>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>PQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>671_A</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>2401.777119828843</v>
+      </c>
+      <c r="C25" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>PQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>675_B</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>2401.777119828843</v>
+      </c>
+      <c r="C26" t="n">
+        <v>1</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>-120</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>PQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>675_C</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>2401.777119828843</v>
+      </c>
+      <c r="C27" t="n">
+        <v>1</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>120</v>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>PQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>675_A</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>2401.777119828843</v>
+      </c>
+      <c r="C28" t="n">
+        <v>1</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>PQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>680_B</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>2401.777119828843</v>
+      </c>
+      <c r="C29" t="n">
+        <v>1</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>-120</v>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>PQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>680_C</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>2401.777119828843</v>
+      </c>
+      <c r="C30" t="n">
+        <v>1</v>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
+        <v>120</v>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>PQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>680_A</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>2401.777119828843</v>
+      </c>
+      <c r="C31" t="n">
+        <v>1</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>PQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>684_C</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>2401.777119828843</v>
+      </c>
+      <c r="C32" t="n">
+        <v>1</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
+        <v>120</v>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>PQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>684_A</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>2401.777119828843</v>
+      </c>
+      <c r="C33" t="n">
+        <v>1</v>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E33" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>PQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>692_B</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>2401.777119828843</v>
+      </c>
+      <c r="C34" t="n">
+        <v>1</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E34" t="n">
+        <v>-120</v>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>PQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>692_C</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>2401.777119828843</v>
+      </c>
+      <c r="C35" t="n">
+        <v>1</v>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E35" t="n">
+        <v>120</v>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>PQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>692_A</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>2401.777119828843</v>
+      </c>
+      <c r="C36" t="n">
+        <v>1</v>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E36" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>PQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>brkr_B</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>2401.777119828843</v>
+      </c>
+      <c r="C37" t="n">
+        <v>1</v>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E37" t="n">
+        <v>-120</v>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>PQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>brkr_C</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>2401.777119828843</v>
+      </c>
+      <c r="C38" t="n">
+        <v>1</v>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E38" t="n">
+        <v>120</v>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>PQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>brkr_A</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>2401.777119828843</v>
+      </c>
+      <c r="C39" t="n">
+        <v>1</v>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E39" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>PQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>house_s1</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>120.0888559914422</v>
+      </c>
+      <c r="C40" t="n">
+        <v>1</v>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E40" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>PQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>house_s2</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>120.0888559914422</v>
+      </c>
+      <c r="C41" t="n">
+        <v>1</v>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E41" t="n">
+        <v>180</v>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>PQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>mid_B</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>2401.777119828843</v>
+      </c>
+      <c r="C42" t="n">
+        <v>1</v>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E42" t="n">
+        <v>-120</v>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>PQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>mid_C</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>2401.777119828843</v>
+      </c>
+      <c r="C43" t="n">
+        <v>1</v>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E43" t="n">
+        <v>120</v>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>PQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>mid_A</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>2401.777119828843</v>
+      </c>
+      <c r="C44" t="n">
+        <v>1</v>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E44" t="n">
+        <v>0</v>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>PQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>rg60_B</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>2401.777119828843</v>
+      </c>
+      <c r="C45" t="n">
+        <v>1</v>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E45" t="n">
+        <v>-120</v>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>PQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>rg60_C</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>2401.777119828843</v>
+      </c>
+      <c r="C46" t="n">
+        <v>1</v>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E46" t="n">
+        <v>120</v>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>PQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>rg60_A</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>2401.777119828843</v>
+      </c>
+      <c r="C47" t="n">
+        <v>1</v>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E47" t="n">
+        <v>0</v>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>PQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>sourcebus_B</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>66395.28095680696</v>
+      </c>
+      <c r="C48" t="n">
+        <v>1</v>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E48" t="n">
+        <v>-120</v>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>SLACK</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>sourcebus_C</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>66395.28095680696</v>
+      </c>
+      <c r="C49" t="n">
+        <v>1</v>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E49" t="n">
+        <v>120</v>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>SLACK</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>sourcebus_A</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>66395.28095680696</v>
+      </c>
+      <c r="C50" t="n">
+        <v>1</v>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E50" t="n">
+        <v>0</v>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>SLACK</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>tap_C</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>2401.777119828843</v>
+      </c>
+      <c r="C51" t="n">
+        <v>1</v>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E51" t="n">
+        <v>120</v>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>PQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>xf1_B</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>2401.777119828843</v>
+      </c>
+      <c r="C52" t="n">
+        <v>1</v>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E52" t="n">
+        <v>-120</v>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>PQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>xf1_C</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>2401.777119828843</v>
+      </c>
+      <c r="C53" t="n">
+        <v>1</v>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E53" t="n">
+        <v>120</v>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>PQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>xf1_A</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>2401.777119828843</v>
+      </c>
+      <c r="C54" t="n">
+        <v>1</v>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E54" t="n">
+        <v>0</v>
+      </c>
+      <c r="F54" t="inlineStr">
         <is>
           <t>PQ</t>
         </is>
@@ -1165,7 +2193,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1198,17 +2226,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>650</t>
+          <t>650_A</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>brkr</t>
+          <t>brkr_A</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>brkr1</t>
+          <t>brkr1_A</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -1218,17 +2246,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>633</t>
+          <t>650_B</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>xf1</t>
+          <t>brkr_B</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>fuse1</t>
+          <t>brkr1_B</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -1238,17 +2266,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>671</t>
+          <t>650_C</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>692</t>
+          <t>brkr_C</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>671692</t>
+          <t>brkr1_C</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -1258,17 +2286,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>684</t>
+          <t>633_A</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>tap</t>
+          <t>xf1_A</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>sect1</t>
+          <t>fuse1_A</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -1278,20 +2306,180 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>632</t>
+          <t>633_B</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>mid</t>
+          <t>xf1_B</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>rec1</t>
+          <t>fuse1_B</t>
         </is>
       </c>
       <c r="D6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>633_C</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>xf1_C</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>fuse1_C</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>671_A</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>692_A</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>671692_A</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>671_B</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>692_B</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>671692_B</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>671_C</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>692_C</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>671692_C</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>684_C</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>tap_C</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>sect1_C</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>632_A</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>mid_A</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>rec1_A</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>632_B</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>mid_B</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>rec1_B</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>632_C</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>mid_C</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>rec1_C</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
filling out headers on all the sheets; had to rename some 2W transformer columns for uniqueness
</commit_message>
<xml_diff>
--- a/CPYDAR/ieee13x.xlsx
+++ b/CPYDAR/ieee13x.xlsx
@@ -9,8 +9,12 @@
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="General" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Voltage Source" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Bus" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Switch" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Load" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Shunt" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Line" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Transformer" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Bus" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Switch" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -764,6 +768,1636 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A11:R33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Positive-Sequence Constant Imepedance Load</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B12" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="C12" s="1" t="inlineStr">
+        <is>
+          <t>Bus</t>
+        </is>
+      </c>
+      <c r="D12" s="1" t="inlineStr">
+        <is>
+          <t>P (MW)</t>
+        </is>
+      </c>
+      <c r="E12" s="1" t="inlineStr">
+        <is>
+          <t>Q (MVAr)</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>End of Positive Sequence Constant Imepedance Load</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Positive-Sequence Constant Power Load</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B16" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="C16" s="1" t="inlineStr">
+        <is>
+          <t>Bus</t>
+        </is>
+      </c>
+      <c r="D16" s="1" t="inlineStr">
+        <is>
+          <t>P (MW)</t>
+        </is>
+      </c>
+      <c r="E16" s="1" t="inlineStr">
+        <is>
+          <t>Q (MVAr)</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>End of Positive Sequence Constant Power Load</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Positive-Sequence Constant Current Load</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B20" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="C20" s="1" t="inlineStr">
+        <is>
+          <t>Bus</t>
+        </is>
+      </c>
+      <c r="D20" s="1" t="inlineStr">
+        <is>
+          <t>P (MW)</t>
+        </is>
+      </c>
+      <c r="E20" s="1" t="inlineStr">
+        <is>
+          <t>Q (MVAr)</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>End of Positive Sequence Constant Current Load</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Single-Phase ZIP Load</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B24" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="C24" s="1" t="inlineStr">
+        <is>
+          <t>V (kV)</t>
+        </is>
+      </c>
+      <c r="D24" s="1" t="inlineStr">
+        <is>
+          <t>Bandwidth (pu)</t>
+        </is>
+      </c>
+      <c r="E24" s="1" t="inlineStr">
+        <is>
+          <t>Conn. type</t>
+        </is>
+      </c>
+      <c r="F24" s="1" t="inlineStr">
+        <is>
+          <t>K_z</t>
+        </is>
+      </c>
+      <c r="G24" s="1" t="inlineStr">
+        <is>
+          <t>K_i</t>
+        </is>
+      </c>
+      <c r="H24" s="1" t="inlineStr">
+        <is>
+          <t>K_p</t>
+        </is>
+      </c>
+      <c r="I24" s="1" t="inlineStr">
+        <is>
+          <t>Use initial voltage?</t>
+        </is>
+      </c>
+      <c r="J24" s="1" t="inlineStr">
+        <is>
+          <t>Bus1</t>
+        </is>
+      </c>
+      <c r="K24" s="1" t="inlineStr">
+        <is>
+          <t>P1 (kW)</t>
+        </is>
+      </c>
+      <c r="L24" s="1" t="inlineStr">
+        <is>
+          <t>Q1 (kVAr)</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>End of SinglePhase ZIP Load</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Two-Phase ZIP Load</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B28" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="C28" s="1" t="inlineStr">
+        <is>
+          <t>V (kV)</t>
+        </is>
+      </c>
+      <c r="D28" s="1" t="inlineStr">
+        <is>
+          <t>Bandwidth (pu)</t>
+        </is>
+      </c>
+      <c r="E28" s="1" t="inlineStr">
+        <is>
+          <t>Conn. type</t>
+        </is>
+      </c>
+      <c r="F28" s="1" t="inlineStr">
+        <is>
+          <t>K_z</t>
+        </is>
+      </c>
+      <c r="G28" s="1" t="inlineStr">
+        <is>
+          <t>K_i</t>
+        </is>
+      </c>
+      <c r="H28" s="1" t="inlineStr">
+        <is>
+          <t>K_p</t>
+        </is>
+      </c>
+      <c r="I28" s="1" t="inlineStr">
+        <is>
+          <t>Use initial voltage?</t>
+        </is>
+      </c>
+      <c r="J28" s="1" t="inlineStr">
+        <is>
+          <t>Bus1</t>
+        </is>
+      </c>
+      <c r="K28" s="1" t="inlineStr">
+        <is>
+          <t>Bus2</t>
+        </is>
+      </c>
+      <c r="L28" s="1" t="inlineStr">
+        <is>
+          <t>P1 (kW)</t>
+        </is>
+      </c>
+      <c r="M28" s="1" t="inlineStr">
+        <is>
+          <t>Q1 (kVAr)</t>
+        </is>
+      </c>
+      <c r="N28" s="1" t="inlineStr">
+        <is>
+          <t>P2 (kW)</t>
+        </is>
+      </c>
+      <c r="O28" s="1" t="inlineStr">
+        <is>
+          <t>Q2 (kVAr)</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>End of TwoPhase ZIP Load</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Three-Phase ZIP Load</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B32" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="C32" s="1" t="inlineStr">
+        <is>
+          <t>V (kV)</t>
+        </is>
+      </c>
+      <c r="D32" s="1" t="inlineStr">
+        <is>
+          <t>Bandwidth (pu)</t>
+        </is>
+      </c>
+      <c r="E32" s="1" t="inlineStr">
+        <is>
+          <t>Conn. type</t>
+        </is>
+      </c>
+      <c r="F32" s="1" t="inlineStr">
+        <is>
+          <t>K_z</t>
+        </is>
+      </c>
+      <c r="G32" s="1" t="inlineStr">
+        <is>
+          <t>K_i</t>
+        </is>
+      </c>
+      <c r="H32" s="1" t="inlineStr">
+        <is>
+          <t>K_p</t>
+        </is>
+      </c>
+      <c r="I32" s="1" t="inlineStr">
+        <is>
+          <t>Use initial voltage?</t>
+        </is>
+      </c>
+      <c r="J32" s="1" t="inlineStr">
+        <is>
+          <t>Bus1</t>
+        </is>
+      </c>
+      <c r="K32" s="1" t="inlineStr">
+        <is>
+          <t>Bus2</t>
+        </is>
+      </c>
+      <c r="L32" s="1" t="inlineStr">
+        <is>
+          <t>Bus3</t>
+        </is>
+      </c>
+      <c r="M32" s="1" t="inlineStr">
+        <is>
+          <t>P1 (kW)</t>
+        </is>
+      </c>
+      <c r="N32" s="1" t="inlineStr">
+        <is>
+          <t>Q1 (kVAr)</t>
+        </is>
+      </c>
+      <c r="O32" s="1" t="inlineStr">
+        <is>
+          <t>P2 (kW)</t>
+        </is>
+      </c>
+      <c r="P32" s="1" t="inlineStr">
+        <is>
+          <t>Q2 (kVAr)</t>
+        </is>
+      </c>
+      <c r="Q32" s="1" t="inlineStr">
+        <is>
+          <t>P3 (kW)</t>
+        </is>
+      </c>
+      <c r="R32" s="1" t="inlineStr">
+        <is>
+          <t>Q3 (kVAr)</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>End of ThreePhase ZIP Load</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A11:N25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Positive Sequence Shunt</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B12" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="C12" s="1" t="inlineStr">
+        <is>
+          <t>Bus</t>
+        </is>
+      </c>
+      <c r="D12" s="1" t="inlineStr">
+        <is>
+          <t>P (MW)</t>
+        </is>
+      </c>
+      <c r="E12" s="1" t="inlineStr">
+        <is>
+          <t>Q (MVAr)</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>End of Positive Sequence Shunt</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Single-Phase Shunt</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B16" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="C16" s="1" t="inlineStr">
+        <is>
+          <t>kV (ph-gr RMS)</t>
+        </is>
+      </c>
+      <c r="D16" s="1" t="inlineStr">
+        <is>
+          <t>Bus1</t>
+        </is>
+      </c>
+      <c r="E16" s="1" t="inlineStr">
+        <is>
+          <t>P1 (kW)</t>
+        </is>
+      </c>
+      <c r="F16" s="1" t="inlineStr">
+        <is>
+          <t>Q1 (kVAr)</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>End of Single-Phase Shunt</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Two-Phase Shunt</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B20" s="1" t="inlineStr">
+        <is>
+          <t>Status1</t>
+        </is>
+      </c>
+      <c r="C20" s="1" t="inlineStr">
+        <is>
+          <t>Status2</t>
+        </is>
+      </c>
+      <c r="D20" s="1" t="inlineStr">
+        <is>
+          <t>kV (ph-gr RMS)</t>
+        </is>
+      </c>
+      <c r="E20" s="1" t="inlineStr">
+        <is>
+          <t>Bus1</t>
+        </is>
+      </c>
+      <c r="F20" s="1" t="inlineStr">
+        <is>
+          <t>Bus2</t>
+        </is>
+      </c>
+      <c r="G20" s="1" t="inlineStr">
+        <is>
+          <t>P1 (kW)</t>
+        </is>
+      </c>
+      <c r="H20" s="1" t="inlineStr">
+        <is>
+          <t>Q1 (kVAr)</t>
+        </is>
+      </c>
+      <c r="I20" s="1" t="inlineStr">
+        <is>
+          <t>P2 (kW)</t>
+        </is>
+      </c>
+      <c r="J20" s="1" t="inlineStr">
+        <is>
+          <t>Q2 (kVAr)</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>End of Two-Phase Shunt</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Three-Phase Shunt</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B24" s="1" t="inlineStr">
+        <is>
+          <t>Status1</t>
+        </is>
+      </c>
+      <c r="C24" s="1" t="inlineStr">
+        <is>
+          <t>Status2</t>
+        </is>
+      </c>
+      <c r="D24" s="1" t="inlineStr">
+        <is>
+          <t>Status3</t>
+        </is>
+      </c>
+      <c r="E24" s="1" t="inlineStr">
+        <is>
+          <t>kV (ph-gr RMS)</t>
+        </is>
+      </c>
+      <c r="F24" s="1" t="inlineStr">
+        <is>
+          <t>Bus1</t>
+        </is>
+      </c>
+      <c r="G24" s="1" t="inlineStr">
+        <is>
+          <t>Bus2</t>
+        </is>
+      </c>
+      <c r="H24" s="1" t="inlineStr">
+        <is>
+          <t>Bus3</t>
+        </is>
+      </c>
+      <c r="I24" s="1" t="inlineStr">
+        <is>
+          <t>P1 (kW)</t>
+        </is>
+      </c>
+      <c r="J24" s="1" t="inlineStr">
+        <is>
+          <t>Q1 (kVAr)</t>
+        </is>
+      </c>
+      <c r="K24" s="1" t="inlineStr">
+        <is>
+          <t>P2 (kW)</t>
+        </is>
+      </c>
+      <c r="L24" s="1" t="inlineStr">
+        <is>
+          <t>Q2 (kVAr)</t>
+        </is>
+      </c>
+      <c r="M24" s="1" t="inlineStr">
+        <is>
+          <t>P3 (kW)</t>
+        </is>
+      </c>
+      <c r="N24" s="1" t="inlineStr">
+        <is>
+          <t>Q3 (kVAr)</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>End of Three-Phase Shunt</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A11:AA29"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Positive-Sequence Line</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B12" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="C12" s="1" t="inlineStr">
+        <is>
+          <t>From bus</t>
+        </is>
+      </c>
+      <c r="D12" s="1" t="inlineStr">
+        <is>
+          <t>To bus</t>
+        </is>
+      </c>
+      <c r="E12" s="1" t="inlineStr">
+        <is>
+          <t>R (pu)</t>
+        </is>
+      </c>
+      <c r="F12" s="1" t="inlineStr">
+        <is>
+          <t>X (pu)</t>
+        </is>
+      </c>
+      <c r="G12" s="1" t="inlineStr">
+        <is>
+          <t>B (pu)</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>End of Positive-Sequence Line</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Single-Phase Line</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B16" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="C16" s="1" t="inlineStr">
+        <is>
+          <t>Length</t>
+        </is>
+      </c>
+      <c r="D16" s="1" t="inlineStr">
+        <is>
+          <t>From1</t>
+        </is>
+      </c>
+      <c r="E16" s="1" t="inlineStr">
+        <is>
+          <t>To1</t>
+        </is>
+      </c>
+      <c r="F16" s="1" t="inlineStr">
+        <is>
+          <t>r11 (Ohm/length_unit)</t>
+        </is>
+      </c>
+      <c r="G16" s="1" t="inlineStr">
+        <is>
+          <t>x11 (Ohm/length_unit)</t>
+        </is>
+      </c>
+      <c r="H16" s="1" t="inlineStr">
+        <is>
+          <t>b11 (uS/length_unit)</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>End of Single-Phase Line</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Two-Phase Line</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B20" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="C20" s="1" t="inlineStr">
+        <is>
+          <t>Length</t>
+        </is>
+      </c>
+      <c r="D20" s="1" t="inlineStr">
+        <is>
+          <t>From1</t>
+        </is>
+      </c>
+      <c r="E20" s="1" t="inlineStr">
+        <is>
+          <t>From2</t>
+        </is>
+      </c>
+      <c r="F20" s="1" t="inlineStr">
+        <is>
+          <t>To1</t>
+        </is>
+      </c>
+      <c r="G20" s="1" t="inlineStr">
+        <is>
+          <t>To2</t>
+        </is>
+      </c>
+      <c r="H20" s="1" t="inlineStr">
+        <is>
+          <t>r11 (Ohm/length_unit)</t>
+        </is>
+      </c>
+      <c r="I20" s="1" t="inlineStr">
+        <is>
+          <t>x11 (Ohm/length_unit)</t>
+        </is>
+      </c>
+      <c r="J20" s="1" t="inlineStr">
+        <is>
+          <t>r21 (Ohm/length_unit)</t>
+        </is>
+      </c>
+      <c r="K20" s="1" t="inlineStr">
+        <is>
+          <t>x21 (Ohm/length_unit)</t>
+        </is>
+      </c>
+      <c r="L20" s="1" t="inlineStr">
+        <is>
+          <t>r22 (Ohm/length_unit)</t>
+        </is>
+      </c>
+      <c r="M20" s="1" t="inlineStr">
+        <is>
+          <t>x22 (Ohm/length_unit)</t>
+        </is>
+      </c>
+      <c r="N20" s="1" t="inlineStr">
+        <is>
+          <t>b11 (uS/length_unit)</t>
+        </is>
+      </c>
+      <c r="O20" s="1" t="inlineStr">
+        <is>
+          <t>b21 (uS/length_unit)</t>
+        </is>
+      </c>
+      <c r="P20" s="1" t="inlineStr">
+        <is>
+          <t>b22 (uS/length_unit)</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>End of Two-Phase Line</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Three-Phase Line with Full Data</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B24" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="C24" s="1" t="inlineStr">
+        <is>
+          <t>Length</t>
+        </is>
+      </c>
+      <c r="D24" s="1" t="inlineStr">
+        <is>
+          <t>From1</t>
+        </is>
+      </c>
+      <c r="E24" s="1" t="inlineStr">
+        <is>
+          <t>From2</t>
+        </is>
+      </c>
+      <c r="F24" s="1" t="inlineStr">
+        <is>
+          <t>From3</t>
+        </is>
+      </c>
+      <c r="G24" s="1" t="inlineStr">
+        <is>
+          <t>To1</t>
+        </is>
+      </c>
+      <c r="H24" s="1" t="inlineStr">
+        <is>
+          <t>To2</t>
+        </is>
+      </c>
+      <c r="I24" s="1" t="inlineStr">
+        <is>
+          <t>To3</t>
+        </is>
+      </c>
+      <c r="J24" s="1" t="inlineStr">
+        <is>
+          <t>r11 (Ohm/length_unit)</t>
+        </is>
+      </c>
+      <c r="K24" s="1" t="inlineStr">
+        <is>
+          <t>x11 (Ohm/length_unit)</t>
+        </is>
+      </c>
+      <c r="L24" s="1" t="inlineStr">
+        <is>
+          <t>r21 (Ohm/length_unit)</t>
+        </is>
+      </c>
+      <c r="M24" s="1" t="inlineStr">
+        <is>
+          <t>x21 (Ohm/length_unit)</t>
+        </is>
+      </c>
+      <c r="N24" s="1" t="inlineStr">
+        <is>
+          <t>r22 (Ohm/length_unit)</t>
+        </is>
+      </c>
+      <c r="O24" s="1" t="inlineStr">
+        <is>
+          <t>x22 (Ohm/length_unit)</t>
+        </is>
+      </c>
+      <c r="P24" s="1" t="inlineStr">
+        <is>
+          <t>r31 (Ohm/length_unit)</t>
+        </is>
+      </c>
+      <c r="Q24" s="1" t="inlineStr">
+        <is>
+          <t>x31 (Ohm/length_unit)</t>
+        </is>
+      </c>
+      <c r="R24" s="1" t="inlineStr">
+        <is>
+          <t>r32 (Ohm/length_unit)</t>
+        </is>
+      </c>
+      <c r="S24" s="1" t="inlineStr">
+        <is>
+          <t>x32 (Ohm/length_unit)</t>
+        </is>
+      </c>
+      <c r="T24" s="1" t="inlineStr">
+        <is>
+          <t>r33 (Ohm/length_unit)</t>
+        </is>
+      </c>
+      <c r="U24" s="1" t="inlineStr">
+        <is>
+          <t>x33 (Ohm/length_unit)</t>
+        </is>
+      </c>
+      <c r="V24" s="1" t="inlineStr">
+        <is>
+          <t>b11 (uS/length_unit)</t>
+        </is>
+      </c>
+      <c r="W24" s="1" t="inlineStr">
+        <is>
+          <t>b21 (uS/length_unit)</t>
+        </is>
+      </c>
+      <c r="X24" s="1" t="inlineStr">
+        <is>
+          <t>b22 (uS/length_unit)</t>
+        </is>
+      </c>
+      <c r="Y24" s="1" t="inlineStr">
+        <is>
+          <t>b31 (uS/length_unit)</t>
+        </is>
+      </c>
+      <c r="Z24" s="1" t="inlineStr">
+        <is>
+          <t>b32 (uS/length_unit)</t>
+        </is>
+      </c>
+      <c r="AA24" s="1" t="inlineStr">
+        <is>
+          <t>b33 (uS/length_unit)</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>End of Three-Phase Line with Full Data</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Three-Phase Line with Sequential Data</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B28" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="C28" s="1" t="inlineStr">
+        <is>
+          <t>Length</t>
+        </is>
+      </c>
+      <c r="D28" s="1" t="inlineStr">
+        <is>
+          <t>From1</t>
+        </is>
+      </c>
+      <c r="E28" s="1" t="inlineStr">
+        <is>
+          <t>From2</t>
+        </is>
+      </c>
+      <c r="F28" s="1" t="inlineStr">
+        <is>
+          <t>From3</t>
+        </is>
+      </c>
+      <c r="G28" s="1" t="inlineStr">
+        <is>
+          <t>To1</t>
+        </is>
+      </c>
+      <c r="H28" s="1" t="inlineStr">
+        <is>
+          <t>To2</t>
+        </is>
+      </c>
+      <c r="I28" s="1" t="inlineStr">
+        <is>
+          <t>To3</t>
+        </is>
+      </c>
+      <c r="J28" s="1" t="inlineStr">
+        <is>
+          <t>R0 (Ohm/length_unit)</t>
+        </is>
+      </c>
+      <c r="K28" s="1" t="inlineStr">
+        <is>
+          <t>X0 (Ohm/length_unit)</t>
+        </is>
+      </c>
+      <c r="L28" s="1" t="inlineStr">
+        <is>
+          <t>R1 (Ohm/length_unit)</t>
+        </is>
+      </c>
+      <c r="M28" s="1" t="inlineStr">
+        <is>
+          <t>X1 (Ohm/length_unit)</t>
+        </is>
+      </c>
+      <c r="N28" s="1" t="inlineStr">
+        <is>
+          <t>B0 (uS/length_unit)</t>
+        </is>
+      </c>
+      <c r="O28" s="1" t="inlineStr">
+        <is>
+          <t>B1 (uS/length_unit)</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>End of Three-Phase Line with Sequential Data</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A11:AA25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Positive-Sequence 2W Transformer</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B12" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="C12" s="1" t="inlineStr">
+        <is>
+          <t>From bus</t>
+        </is>
+      </c>
+      <c r="D12" s="1" t="inlineStr">
+        <is>
+          <t>To bus</t>
+        </is>
+      </c>
+      <c r="E12" s="1" t="inlineStr">
+        <is>
+          <t>R (pu)</t>
+        </is>
+      </c>
+      <c r="F12" s="1" t="inlineStr">
+        <is>
+          <t>Xl (pu)</t>
+        </is>
+      </c>
+      <c r="G12" s="1" t="inlineStr">
+        <is>
+          <t>Gmag (pu)</t>
+        </is>
+      </c>
+      <c r="H12" s="1" t="inlineStr">
+        <is>
+          <t>Bmag (pu)</t>
+        </is>
+      </c>
+      <c r="I12" s="1" t="inlineStr">
+        <is>
+          <t>Ratio W1 (pu)</t>
+        </is>
+      </c>
+      <c r="J12" s="1" t="inlineStr">
+        <is>
+          <t>Ratio W2 (pu)</t>
+        </is>
+      </c>
+      <c r="K12" s="1" t="inlineStr">
+        <is>
+          <t>Phase Shift (deg)</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>End of Positive-Sequence 2W Transformer</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Positive-Sequence 3W Transformer</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B16" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="C16" s="1" t="inlineStr">
+        <is>
+          <t>Bus1</t>
+        </is>
+      </c>
+      <c r="D16" s="1" t="inlineStr">
+        <is>
+          <t>Bus2</t>
+        </is>
+      </c>
+      <c r="E16" s="1" t="inlineStr">
+        <is>
+          <t>Bus3</t>
+        </is>
+      </c>
+      <c r="F16" s="1" t="inlineStr">
+        <is>
+          <t>R_12 (pu)</t>
+        </is>
+      </c>
+      <c r="G16" s="1" t="inlineStr">
+        <is>
+          <t>Xl_12 (pu)</t>
+        </is>
+      </c>
+      <c r="H16" s="1" t="inlineStr">
+        <is>
+          <t>R_23 (pu)</t>
+        </is>
+      </c>
+      <c r="I16" s="1" t="inlineStr">
+        <is>
+          <t>Xl_23 (pu)</t>
+        </is>
+      </c>
+      <c r="J16" s="1" t="inlineStr">
+        <is>
+          <t>R_31 (pu)</t>
+        </is>
+      </c>
+      <c r="K16" s="1" t="inlineStr">
+        <is>
+          <t>Xl_31 (pu)</t>
+        </is>
+      </c>
+      <c r="L16" s="1" t="inlineStr">
+        <is>
+          <t>Gmag (pu)</t>
+        </is>
+      </c>
+      <c r="M16" s="1" t="inlineStr">
+        <is>
+          <t>Bmag (pu)</t>
+        </is>
+      </c>
+      <c r="N16" s="1" t="inlineStr">
+        <is>
+          <t>Ratio W1 (pu)</t>
+        </is>
+      </c>
+      <c r="O16" s="1" t="inlineStr">
+        <is>
+          <t>Ratio W2 (pu)</t>
+        </is>
+      </c>
+      <c r="P16" s="1" t="inlineStr">
+        <is>
+          <t>Ratio W3 (pu)</t>
+        </is>
+      </c>
+      <c r="Q16" s="1" t="inlineStr">
+        <is>
+          <t>Phase Shift W1 (deg)</t>
+        </is>
+      </c>
+      <c r="R16" s="1" t="inlineStr">
+        <is>
+          <t>Phase Shift W2 (deg)</t>
+        </is>
+      </c>
+      <c r="S16" s="1" t="inlineStr">
+        <is>
+          <t>Phase Shift W3 (deg)</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>End of Positive-Sequence 3W Transformer</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Multiphase 2W Transformer</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B20" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="C20" s="1" t="inlineStr">
+        <is>
+          <t>Number of phases</t>
+        </is>
+      </c>
+      <c r="D20" s="1" t="inlineStr">
+        <is>
+          <t>Bus1_A</t>
+        </is>
+      </c>
+      <c r="E20" s="1" t="inlineStr">
+        <is>
+          <t>Bus1_B</t>
+        </is>
+      </c>
+      <c r="F20" s="1" t="inlineStr">
+        <is>
+          <t>Bus1_C</t>
+        </is>
+      </c>
+      <c r="G20" s="1" t="inlineStr">
+        <is>
+          <t>V1 (kV)</t>
+        </is>
+      </c>
+      <c r="H20" s="1" t="inlineStr">
+        <is>
+          <t>S_base1 (kVA)</t>
+        </is>
+      </c>
+      <c r="I20" s="1" t="inlineStr">
+        <is>
+          <t>Conn. type1</t>
+        </is>
+      </c>
+      <c r="J20" s="1" t="inlineStr">
+        <is>
+          <t>Bus2_A</t>
+        </is>
+      </c>
+      <c r="K20" s="1" t="inlineStr">
+        <is>
+          <t>Bus2_B</t>
+        </is>
+      </c>
+      <c r="L20" s="1" t="inlineStr">
+        <is>
+          <t>Bus2_C</t>
+        </is>
+      </c>
+      <c r="M20" s="1" t="inlineStr">
+        <is>
+          <t>V2 (kV)</t>
+        </is>
+      </c>
+      <c r="N20" s="1" t="inlineStr">
+        <is>
+          <t>S_base2 (kVA)</t>
+        </is>
+      </c>
+      <c r="O20" s="1" t="inlineStr">
+        <is>
+          <t>Conn. type2</t>
+        </is>
+      </c>
+      <c r="P20" s="1" t="inlineStr">
+        <is>
+          <t>Tap 1</t>
+        </is>
+      </c>
+      <c r="Q20" s="1" t="inlineStr">
+        <is>
+          <t>Tap 2</t>
+        </is>
+      </c>
+      <c r="R20" s="1" t="inlineStr">
+        <is>
+          <t>Tap 3</t>
+        </is>
+      </c>
+      <c r="S20" s="1" t="inlineStr">
+        <is>
+          <t>Lowest Tap</t>
+        </is>
+      </c>
+      <c r="T20" s="1" t="inlineStr">
+        <is>
+          <t>Highest Tap</t>
+        </is>
+      </c>
+      <c r="U20" s="1" t="inlineStr">
+        <is>
+          <t>Min Range (%)</t>
+        </is>
+      </c>
+      <c r="V20" s="1" t="inlineStr">
+        <is>
+          <t>Max Range (%)</t>
+        </is>
+      </c>
+      <c r="W20" s="1" t="inlineStr">
+        <is>
+          <t>X (pu)</t>
+        </is>
+      </c>
+      <c r="X20" s="1" t="inlineStr">
+        <is>
+          <t>RW1 (pu)</t>
+        </is>
+      </c>
+      <c r="Y20" s="1" t="inlineStr">
+        <is>
+          <t>RW2</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>End of Multiphase 2W Transformer</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Multiphase 2W Transformer with Mutual Impedance</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B24" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="C24" s="1" t="inlineStr">
+        <is>
+          <t>Number of phases</t>
+        </is>
+      </c>
+      <c r="D24" s="1" t="inlineStr">
+        <is>
+          <t>Bus1_A</t>
+        </is>
+      </c>
+      <c r="E24" s="1" t="inlineStr">
+        <is>
+          <t>Bus1_B</t>
+        </is>
+      </c>
+      <c r="F24" s="1" t="inlineStr">
+        <is>
+          <t>Bus1_C</t>
+        </is>
+      </c>
+      <c r="G24" s="1" t="inlineStr">
+        <is>
+          <t>V1 (kV)</t>
+        </is>
+      </c>
+      <c r="H24" s="1" t="inlineStr">
+        <is>
+          <t>S_base1 (kVA)</t>
+        </is>
+      </c>
+      <c r="I24" s="1" t="inlineStr">
+        <is>
+          <t>Conn. type1</t>
+        </is>
+      </c>
+      <c r="J24" s="1" t="inlineStr">
+        <is>
+          <t>Bus2_A</t>
+        </is>
+      </c>
+      <c r="K24" s="1" t="inlineStr">
+        <is>
+          <t>Bus2_B</t>
+        </is>
+      </c>
+      <c r="L24" s="1" t="inlineStr">
+        <is>
+          <t>Bus2_C</t>
+        </is>
+      </c>
+      <c r="M24" s="1" t="inlineStr">
+        <is>
+          <t>V2 (kV)</t>
+        </is>
+      </c>
+      <c r="N24" s="1" t="inlineStr">
+        <is>
+          <t>S_base2 (kVA)</t>
+        </is>
+      </c>
+      <c r="O24" s="1" t="inlineStr">
+        <is>
+          <t>Conn. type2</t>
+        </is>
+      </c>
+      <c r="P24" s="1" t="inlineStr">
+        <is>
+          <t>Tap 1</t>
+        </is>
+      </c>
+      <c r="Q24" s="1" t="inlineStr">
+        <is>
+          <t>Tap 2</t>
+        </is>
+      </c>
+      <c r="R24" s="1" t="inlineStr">
+        <is>
+          <t>Tap 3</t>
+        </is>
+      </c>
+      <c r="S24" s="1" t="inlineStr">
+        <is>
+          <t>Lowest Tap</t>
+        </is>
+      </c>
+      <c r="T24" s="1" t="inlineStr">
+        <is>
+          <t>Highest Tap</t>
+        </is>
+      </c>
+      <c r="U24" s="1" t="inlineStr">
+        <is>
+          <t>Min Range (%)</t>
+        </is>
+      </c>
+      <c r="V24" s="1" t="inlineStr">
+        <is>
+          <t>Max Range (%)</t>
+        </is>
+      </c>
+      <c r="W24" s="1" t="inlineStr">
+        <is>
+          <t>Z0 leakage (pu)</t>
+        </is>
+      </c>
+      <c r="X24" s="1" t="inlineStr">
+        <is>
+          <t>Z1 leakage (pu)</t>
+        </is>
+      </c>
+      <c r="Y24" s="1" t="inlineStr">
+        <is>
+          <t>X0/R0</t>
+        </is>
+      </c>
+      <c r="Z24" s="1" t="inlineStr">
+        <is>
+          <t>X1/R1</t>
+        </is>
+      </c>
+      <c r="AA24" s="1" t="inlineStr">
+        <is>
+          <t>No Load Loss (kW)</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>End of Multiphase 2W Transformer with Mutual Impedance</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -859,7 +2493,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>632_C</t>
+          <t>632_A</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -874,7 +2508,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -885,7 +2519,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>632_A</t>
+          <t>632_C</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -900,7 +2534,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -937,7 +2571,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>633_C</t>
+          <t>633_A</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -952,7 +2586,7 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -963,7 +2597,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>633_A</t>
+          <t>633_C</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -978,7 +2612,7 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -1015,7 +2649,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>634_C</t>
+          <t>634_A</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -1030,7 +2664,7 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -1041,7 +2675,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>634_A</t>
+          <t>634_C</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -1056,7 +2690,7 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -1197,7 +2831,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>650_C</t>
+          <t>650_A</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -1212,7 +2846,7 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -1223,7 +2857,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>650_A</t>
+          <t>650_C</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -1238,7 +2872,7 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
@@ -1301,7 +2935,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>670_C</t>
+          <t>670_A</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -1316,7 +2950,7 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
@@ -1327,7 +2961,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>670_A</t>
+          <t>670_C</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -1342,7 +2976,7 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
@@ -1379,7 +3013,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>671_C</t>
+          <t>671_A</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -1394,7 +3028,7 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
@@ -1405,7 +3039,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>671_A</t>
+          <t>671_C</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -1420,7 +3054,7 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -1457,7 +3091,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>675_C</t>
+          <t>675_A</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -1472,7 +3106,7 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
@@ -1483,7 +3117,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>675_A</t>
+          <t>675_C</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -1498,7 +3132,7 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
@@ -1535,7 +3169,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>680_C</t>
+          <t>680_A</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -1550,7 +3184,7 @@
         </is>
       </c>
       <c r="E30" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
@@ -1561,7 +3195,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>680_A</t>
+          <t>680_C</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -1576,7 +3210,7 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
@@ -1587,7 +3221,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>684_C</t>
+          <t>684_A</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -1602,7 +3236,7 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
@@ -1613,7 +3247,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>684_A</t>
+          <t>684_C</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -1628,7 +3262,7 @@
         </is>
       </c>
       <c r="E33" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
@@ -1665,7 +3299,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>692_C</t>
+          <t>692_A</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -1680,7 +3314,7 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
@@ -1691,7 +3325,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>692_A</t>
+          <t>692_C</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -1706,7 +3340,7 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
@@ -1743,7 +3377,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>brkr_C</t>
+          <t>brkr_A</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -1758,7 +3392,7 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
@@ -1769,7 +3403,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>brkr_A</t>
+          <t>brkr_C</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -1784,7 +3418,7 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
@@ -1795,7 +3429,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>house_s1</t>
+          <t>house_s2</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -1810,7 +3444,7 @@
         </is>
       </c>
       <c r="E40" t="n">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
@@ -1821,7 +3455,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>house_s2</t>
+          <t>house_s1</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -1836,7 +3470,7 @@
         </is>
       </c>
       <c r="E41" t="n">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
@@ -1873,7 +3507,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>mid_C</t>
+          <t>mid_A</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -1888,7 +3522,7 @@
         </is>
       </c>
       <c r="E43" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
@@ -1899,7 +3533,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>mid_A</t>
+          <t>mid_C</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -1914,7 +3548,7 @@
         </is>
       </c>
       <c r="E44" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
@@ -1951,7 +3585,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>rg60_C</t>
+          <t>rg60_A</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -1966,7 +3600,7 @@
         </is>
       </c>
       <c r="E46" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
@@ -1977,7 +3611,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>rg60_A</t>
+          <t>rg60_C</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -1992,7 +3626,7 @@
         </is>
       </c>
       <c r="E47" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
@@ -2029,7 +3663,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>sourcebus_C</t>
+          <t>sourcebus_A</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -2044,7 +3678,7 @@
         </is>
       </c>
       <c r="E49" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
@@ -2055,7 +3689,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>sourcebus_A</t>
+          <t>sourcebus_C</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -2070,7 +3704,7 @@
         </is>
       </c>
       <c r="E50" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
@@ -2133,7 +3767,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>xf1_C</t>
+          <t>xf1_A</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -2148,7 +3782,7 @@
         </is>
       </c>
       <c r="E53" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F53" t="inlineStr">
         <is>
@@ -2159,7 +3793,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>xf1_A</t>
+          <t>xf1_C</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -2174,7 +3808,7 @@
         </is>
       </c>
       <c r="E54" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>
@@ -2187,7 +3821,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
keeping track of Excel insertion row
</commit_message>
<xml_diff>
--- a/CPYDAR/ieee13x.xlsx
+++ b/CPYDAR/ieee13x.xlsx
@@ -2493,7 +2493,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>632_A</t>
+          <t>632_C</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -2508,7 +2508,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -2519,7 +2519,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>632_C</t>
+          <t>632_A</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -2534,7 +2534,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -2571,7 +2571,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>633_A</t>
+          <t>633_C</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -2586,7 +2586,7 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -2597,7 +2597,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>633_C</t>
+          <t>633_A</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -2612,7 +2612,7 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -2649,7 +2649,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>634_A</t>
+          <t>634_C</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -2664,7 +2664,7 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -2675,7 +2675,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>634_C</t>
+          <t>634_A</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -2690,7 +2690,7 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -2831,7 +2831,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>650_A</t>
+          <t>650_C</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -2846,7 +2846,7 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -2857,7 +2857,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>650_C</t>
+          <t>650_A</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -2872,7 +2872,7 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
@@ -2935,7 +2935,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>670_A</t>
+          <t>670_C</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -2950,7 +2950,7 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
@@ -2961,7 +2961,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>670_C</t>
+          <t>670_A</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -2976,7 +2976,7 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
@@ -3013,7 +3013,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>671_A</t>
+          <t>671_C</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -3028,7 +3028,7 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
@@ -3039,7 +3039,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>671_C</t>
+          <t>671_A</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -3054,7 +3054,7 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -3091,7 +3091,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>675_A</t>
+          <t>675_C</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -3106,7 +3106,7 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
@@ -3117,7 +3117,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>675_C</t>
+          <t>675_A</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -3132,7 +3132,7 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
@@ -3169,7 +3169,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>680_A</t>
+          <t>680_C</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -3184,7 +3184,7 @@
         </is>
       </c>
       <c r="E30" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
@@ -3195,7 +3195,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>680_C</t>
+          <t>680_A</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -3210,7 +3210,7 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
@@ -3221,7 +3221,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>684_A</t>
+          <t>684_C</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -3236,7 +3236,7 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
@@ -3247,7 +3247,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>684_C</t>
+          <t>684_A</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -3262,7 +3262,7 @@
         </is>
       </c>
       <c r="E33" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
@@ -3299,7 +3299,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>692_A</t>
+          <t>692_C</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -3314,7 +3314,7 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
@@ -3325,7 +3325,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>692_C</t>
+          <t>692_A</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -3340,7 +3340,7 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
@@ -3377,7 +3377,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>brkr_A</t>
+          <t>brkr_C</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -3392,7 +3392,7 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
@@ -3403,7 +3403,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>brkr_C</t>
+          <t>brkr_A</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -3418,7 +3418,7 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
@@ -3507,7 +3507,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>mid_A</t>
+          <t>mid_C</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -3522,7 +3522,7 @@
         </is>
       </c>
       <c r="E43" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
@@ -3533,7 +3533,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>mid_C</t>
+          <t>mid_A</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -3548,7 +3548,7 @@
         </is>
       </c>
       <c r="E44" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
@@ -3585,7 +3585,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>rg60_A</t>
+          <t>rg60_C</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -3600,7 +3600,7 @@
         </is>
       </c>
       <c r="E46" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
@@ -3611,7 +3611,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>rg60_C</t>
+          <t>rg60_A</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -3626,7 +3626,7 @@
         </is>
       </c>
       <c r="E47" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
@@ -3663,7 +3663,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>sourcebus_A</t>
+          <t>sourcebus_C</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -3678,7 +3678,7 @@
         </is>
       </c>
       <c r="E49" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
@@ -3689,7 +3689,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>sourcebus_C</t>
+          <t>sourcebus_A</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -3704,7 +3704,7 @@
         </is>
       </c>
       <c r="E50" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
@@ -3767,7 +3767,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>xf1_A</t>
+          <t>xf1_C</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -3782,7 +3782,7 @@
         </is>
       </c>
       <c r="E53" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F53" t="inlineStr">
         <is>
@@ -3793,7 +3793,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>xf1_C</t>
+          <t>xf1_A</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -3808,7 +3808,7 @@
         </is>
       </c>
       <c r="E54" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
implemented loads, DER, and capacitors
</commit_message>
<xml_diff>
--- a/CPYDAR/ieee13x.xlsx
+++ b/CPYDAR/ieee13x.xlsx
@@ -768,7 +768,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A11:R33"/>
+  <dimension ref="A11:R53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -971,202 +971,1181 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>End of SinglePhase ZIP Load</t>
-        </is>
+          <t>611</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>1</v>
+      </c>
+      <c r="C25" t="n">
+        <v>4.16</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>wye</t>
+        </is>
+      </c>
+      <c r="F25" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" t="n">
+        <v>100</v>
+      </c>
+      <c r="H25" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0</v>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>611_C</t>
+        </is>
+      </c>
+      <c r="K25" t="n">
+        <v>170</v>
+      </c>
+      <c r="L25" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>634a</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>1</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>wye</t>
+        </is>
+      </c>
+      <c r="F26" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" t="n">
+        <v>100</v>
+      </c>
+      <c r="I26" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>634_A</t>
+        </is>
+      </c>
+      <c r="K26" t="n">
+        <v>160</v>
+      </c>
+      <c r="L26" t="n">
+        <v>110</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Two-Phase ZIP Load</t>
-        </is>
+          <t>634b</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>1</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>wye</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" t="n">
+        <v>100</v>
+      </c>
+      <c r="I27" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>634_B</t>
+        </is>
+      </c>
+      <c r="K27" t="n">
+        <v>120</v>
+      </c>
+      <c r="L27" t="n">
+        <v>90</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="1" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="B28" s="1" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
-      </c>
-      <c r="C28" s="1" t="inlineStr">
-        <is>
-          <t>V (kV)</t>
-        </is>
-      </c>
-      <c r="D28" s="1" t="inlineStr">
-        <is>
-          <t>Bandwidth (pu)</t>
-        </is>
-      </c>
-      <c r="E28" s="1" t="inlineStr">
-        <is>
-          <t>Conn. type</t>
-        </is>
-      </c>
-      <c r="F28" s="1" t="inlineStr">
-        <is>
-          <t>K_z</t>
-        </is>
-      </c>
-      <c r="G28" s="1" t="inlineStr">
-        <is>
-          <t>K_i</t>
-        </is>
-      </c>
-      <c r="H28" s="1" t="inlineStr">
-        <is>
-          <t>K_p</t>
-        </is>
-      </c>
-      <c r="I28" s="1" t="inlineStr">
-        <is>
-          <t>Use initial voltage?</t>
-        </is>
-      </c>
-      <c r="J28" s="1" t="inlineStr">
-        <is>
-          <t>Bus1</t>
-        </is>
-      </c>
-      <c r="K28" s="1" t="inlineStr">
-        <is>
-          <t>Bus2</t>
-        </is>
-      </c>
-      <c r="L28" s="1" t="inlineStr">
-        <is>
-          <t>P1 (kW)</t>
-        </is>
-      </c>
-      <c r="M28" s="1" t="inlineStr">
-        <is>
-          <t>Q1 (kVAr)</t>
-        </is>
-      </c>
-      <c r="N28" s="1" t="inlineStr">
-        <is>
-          <t>P2 (kW)</t>
-        </is>
-      </c>
-      <c r="O28" s="1" t="inlineStr">
-        <is>
-          <t>Q2 (kVAr)</t>
-        </is>
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>634c</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>1</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>wye</t>
+        </is>
+      </c>
+      <c r="F28" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" t="n">
+        <v>100</v>
+      </c>
+      <c r="I28" t="n">
+        <v>0</v>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>634_C</t>
+        </is>
+      </c>
+      <c r="K28" t="n">
+        <v>120</v>
+      </c>
+      <c r="L28" t="n">
+        <v>90</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>End of TwoPhase ZIP Load</t>
-        </is>
+          <t>645</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>1</v>
+      </c>
+      <c r="C29" t="n">
+        <v>4.16</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>wye</t>
+        </is>
+      </c>
+      <c r="F29" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0</v>
+      </c>
+      <c r="H29" t="n">
+        <v>100</v>
+      </c>
+      <c r="I29" t="n">
+        <v>0</v>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>645_B</t>
+        </is>
+      </c>
+      <c r="K29" t="n">
+        <v>170</v>
+      </c>
+      <c r="L29" t="n">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>646</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>1</v>
+      </c>
+      <c r="C30" t="n">
+        <v>4.16</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>delta</t>
+        </is>
+      </c>
+      <c r="F30" t="n">
+        <v>100</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0</v>
+      </c>
+      <c r="H30" t="n">
+        <v>0</v>
+      </c>
+      <c r="I30" t="n">
+        <v>0</v>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>646_B</t>
+        </is>
+      </c>
+      <c r="K30" t="n">
+        <v>230</v>
+      </c>
+      <c r="L30" t="n">
+        <v>132</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Three-Phase ZIP Load</t>
-        </is>
+          <t>652</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>1</v>
+      </c>
+      <c r="C31" t="n">
+        <v>4.16</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>wye</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
+        <v>100</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0</v>
+      </c>
+      <c r="H31" t="n">
+        <v>0</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0</v>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>652_A</t>
+        </is>
+      </c>
+      <c r="K31" t="n">
+        <v>128</v>
+      </c>
+      <c r="L31" t="n">
+        <v>86</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="1" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="B32" s="1" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
-      </c>
-      <c r="C32" s="1" t="inlineStr">
-        <is>
-          <t>V (kV)</t>
-        </is>
-      </c>
-      <c r="D32" s="1" t="inlineStr">
-        <is>
-          <t>Bandwidth (pu)</t>
-        </is>
-      </c>
-      <c r="E32" s="1" t="inlineStr">
-        <is>
-          <t>Conn. type</t>
-        </is>
-      </c>
-      <c r="F32" s="1" t="inlineStr">
-        <is>
-          <t>K_z</t>
-        </is>
-      </c>
-      <c r="G32" s="1" t="inlineStr">
-        <is>
-          <t>K_i</t>
-        </is>
-      </c>
-      <c r="H32" s="1" t="inlineStr">
-        <is>
-          <t>K_p</t>
-        </is>
-      </c>
-      <c r="I32" s="1" t="inlineStr">
-        <is>
-          <t>Use initial voltage?</t>
-        </is>
-      </c>
-      <c r="J32" s="1" t="inlineStr">
-        <is>
-          <t>Bus1</t>
-        </is>
-      </c>
-      <c r="K32" s="1" t="inlineStr">
-        <is>
-          <t>Bus2</t>
-        </is>
-      </c>
-      <c r="L32" s="1" t="inlineStr">
-        <is>
-          <t>Bus3</t>
-        </is>
-      </c>
-      <c r="M32" s="1" t="inlineStr">
-        <is>
-          <t>P1 (kW)</t>
-        </is>
-      </c>
-      <c r="N32" s="1" t="inlineStr">
-        <is>
-          <t>Q1 (kVAr)</t>
-        </is>
-      </c>
-      <c r="O32" s="1" t="inlineStr">
-        <is>
-          <t>P2 (kW)</t>
-        </is>
-      </c>
-      <c r="P32" s="1" t="inlineStr">
-        <is>
-          <t>Q2 (kVAr)</t>
-        </is>
-      </c>
-      <c r="Q32" s="1" t="inlineStr">
-        <is>
-          <t>P3 (kW)</t>
-        </is>
-      </c>
-      <c r="R32" s="1" t="inlineStr">
-        <is>
-          <t>Q3 (kVAr)</t>
-        </is>
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>670a</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>1</v>
+      </c>
+      <c r="C32" t="n">
+        <v>4.16</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>wye</t>
+        </is>
+      </c>
+      <c r="F32" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0</v>
+      </c>
+      <c r="H32" t="n">
+        <v>100</v>
+      </c>
+      <c r="I32" t="n">
+        <v>0</v>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>670_A</t>
+        </is>
+      </c>
+      <c r="K32" t="n">
+        <v>17</v>
+      </c>
+      <c r="L32" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
+        <is>
+          <t>670b</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>1</v>
+      </c>
+      <c r="C33" t="n">
+        <v>4.16</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>wye</t>
+        </is>
+      </c>
+      <c r="F33" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0</v>
+      </c>
+      <c r="H33" t="n">
+        <v>100</v>
+      </c>
+      <c r="I33" t="n">
+        <v>0</v>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>670_B</t>
+        </is>
+      </c>
+      <c r="K33" t="n">
+        <v>66</v>
+      </c>
+      <c r="L33" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>670c</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>1</v>
+      </c>
+      <c r="C34" t="n">
+        <v>4.16</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>wye</t>
+        </is>
+      </c>
+      <c r="F34" t="n">
+        <v>0</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0</v>
+      </c>
+      <c r="H34" t="n">
+        <v>100</v>
+      </c>
+      <c r="I34" t="n">
+        <v>0</v>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>670_C</t>
+        </is>
+      </c>
+      <c r="K34" t="n">
+        <v>117</v>
+      </c>
+      <c r="L34" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>675a</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>1</v>
+      </c>
+      <c r="C35" t="n">
+        <v>4.16</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>wye</t>
+        </is>
+      </c>
+      <c r="F35" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0</v>
+      </c>
+      <c r="H35" t="n">
+        <v>100</v>
+      </c>
+      <c r="I35" t="n">
+        <v>0</v>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>675_A</t>
+        </is>
+      </c>
+      <c r="K35" t="n">
+        <v>485</v>
+      </c>
+      <c r="L35" t="n">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>675b</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>1</v>
+      </c>
+      <c r="C36" t="n">
+        <v>4.16</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>wye</t>
+        </is>
+      </c>
+      <c r="F36" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" t="n">
+        <v>0</v>
+      </c>
+      <c r="H36" t="n">
+        <v>100</v>
+      </c>
+      <c r="I36" t="n">
+        <v>0</v>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>675_B</t>
+        </is>
+      </c>
+      <c r="K36" t="n">
+        <v>68</v>
+      </c>
+      <c r="L36" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>675c</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>1</v>
+      </c>
+      <c r="C37" t="n">
+        <v>4.16</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>wye</t>
+        </is>
+      </c>
+      <c r="F37" t="n">
+        <v>0</v>
+      </c>
+      <c r="G37" t="n">
+        <v>0</v>
+      </c>
+      <c r="H37" t="n">
+        <v>100</v>
+      </c>
+      <c r="I37" t="n">
+        <v>0</v>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>675_C</t>
+        </is>
+      </c>
+      <c r="K37" t="n">
+        <v>290</v>
+      </c>
+      <c r="L37" t="n">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>692</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>1</v>
+      </c>
+      <c r="C38" t="n">
+        <v>4.16</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>delta</t>
+        </is>
+      </c>
+      <c r="F38" t="n">
+        <v>0</v>
+      </c>
+      <c r="G38" t="n">
+        <v>100</v>
+      </c>
+      <c r="H38" t="n">
+        <v>0</v>
+      </c>
+      <c r="I38" t="n">
+        <v>0</v>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>692_C</t>
+        </is>
+      </c>
+      <c r="K38" t="n">
+        <v>170</v>
+      </c>
+      <c r="L38" t="n">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>End of SinglePhase ZIP Load</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Two-Phase ZIP Load</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B42" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="C42" s="1" t="inlineStr">
+        <is>
+          <t>V (kV)</t>
+        </is>
+      </c>
+      <c r="D42" s="1" t="inlineStr">
+        <is>
+          <t>Bandwidth (pu)</t>
+        </is>
+      </c>
+      <c r="E42" s="1" t="inlineStr">
+        <is>
+          <t>Conn. type</t>
+        </is>
+      </c>
+      <c r="F42" s="1" t="inlineStr">
+        <is>
+          <t>K_z</t>
+        </is>
+      </c>
+      <c r="G42" s="1" t="inlineStr">
+        <is>
+          <t>K_i</t>
+        </is>
+      </c>
+      <c r="H42" s="1" t="inlineStr">
+        <is>
+          <t>K_p</t>
+        </is>
+      </c>
+      <c r="I42" s="1" t="inlineStr">
+        <is>
+          <t>Use initial voltage?</t>
+        </is>
+      </c>
+      <c r="J42" s="1" t="inlineStr">
+        <is>
+          <t>Bus1</t>
+        </is>
+      </c>
+      <c r="K42" s="1" t="inlineStr">
+        <is>
+          <t>Bus2</t>
+        </is>
+      </c>
+      <c r="L42" s="1" t="inlineStr">
+        <is>
+          <t>P1 (kW)</t>
+        </is>
+      </c>
+      <c r="M42" s="1" t="inlineStr">
+        <is>
+          <t>Q1 (kVAr)</t>
+        </is>
+      </c>
+      <c r="N42" s="1" t="inlineStr">
+        <is>
+          <t>P2 (kW)</t>
+        </is>
+      </c>
+      <c r="O42" s="1" t="inlineStr">
+        <is>
+          <t>Q2 (kVAr)</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>house</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>1</v>
+      </c>
+      <c r="C43" t="n">
+        <v>0.208</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>wye</t>
+        </is>
+      </c>
+      <c r="F43" t="n">
+        <v>0</v>
+      </c>
+      <c r="G43" t="n">
+        <v>0</v>
+      </c>
+      <c r="H43" t="n">
+        <v>100</v>
+      </c>
+      <c r="I43" t="n">
+        <v>0</v>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>house_s1</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>house_s2</t>
+        </is>
+      </c>
+      <c r="L43" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="M43" t="n">
+        <v>1.54936085</v>
+      </c>
+      <c r="N43" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="O43" t="n">
+        <v>1.54936085</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>pv_house</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>1</v>
+      </c>
+      <c r="C44" t="n">
+        <v>0.208</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>wye</t>
+        </is>
+      </c>
+      <c r="F44" t="n">
+        <v>0</v>
+      </c>
+      <c r="G44" t="n">
+        <v>100</v>
+      </c>
+      <c r="H44" t="n">
+        <v>0</v>
+      </c>
+      <c r="I44" t="n">
+        <v>0</v>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>house_s1</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>house_s2</t>
+        </is>
+      </c>
+      <c r="L44" t="n">
+        <v>-2</v>
+      </c>
+      <c r="M44" t="n">
+        <v>-0</v>
+      </c>
+      <c r="N44" t="n">
+        <v>-2</v>
+      </c>
+      <c r="O44" t="n">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>bat_house</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>1</v>
+      </c>
+      <c r="C45" t="n">
+        <v>0.208</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>wye</t>
+        </is>
+      </c>
+      <c r="F45" t="n">
+        <v>0</v>
+      </c>
+      <c r="G45" t="n">
+        <v>100</v>
+      </c>
+      <c r="H45" t="n">
+        <v>0</v>
+      </c>
+      <c r="I45" t="n">
+        <v>0</v>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>house_s1</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>house_s2</t>
+        </is>
+      </c>
+      <c r="L45" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="M45" t="n">
+        <v>-0</v>
+      </c>
+      <c r="N45" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="O45" t="n">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>End of TwoPhase ZIP Load</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Three-Phase ZIP Load</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B49" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="C49" s="1" t="inlineStr">
+        <is>
+          <t>V (kV)</t>
+        </is>
+      </c>
+      <c r="D49" s="1" t="inlineStr">
+        <is>
+          <t>Bandwidth (pu)</t>
+        </is>
+      </c>
+      <c r="E49" s="1" t="inlineStr">
+        <is>
+          <t>Conn. type</t>
+        </is>
+      </c>
+      <c r="F49" s="1" t="inlineStr">
+        <is>
+          <t>K_z</t>
+        </is>
+      </c>
+      <c r="G49" s="1" t="inlineStr">
+        <is>
+          <t>K_i</t>
+        </is>
+      </c>
+      <c r="H49" s="1" t="inlineStr">
+        <is>
+          <t>K_p</t>
+        </is>
+      </c>
+      <c r="I49" s="1" t="inlineStr">
+        <is>
+          <t>Use initial voltage?</t>
+        </is>
+      </c>
+      <c r="J49" s="1" t="inlineStr">
+        <is>
+          <t>Bus1</t>
+        </is>
+      </c>
+      <c r="K49" s="1" t="inlineStr">
+        <is>
+          <t>Bus2</t>
+        </is>
+      </c>
+      <c r="L49" s="1" t="inlineStr">
+        <is>
+          <t>Bus3</t>
+        </is>
+      </c>
+      <c r="M49" s="1" t="inlineStr">
+        <is>
+          <t>P1 (kW)</t>
+        </is>
+      </c>
+      <c r="N49" s="1" t="inlineStr">
+        <is>
+          <t>Q1 (kVAr)</t>
+        </is>
+      </c>
+      <c r="O49" s="1" t="inlineStr">
+        <is>
+          <t>P2 (kW)</t>
+        </is>
+      </c>
+      <c r="P49" s="1" t="inlineStr">
+        <is>
+          <t>Q2 (kVAr)</t>
+        </is>
+      </c>
+      <c r="Q49" s="1" t="inlineStr">
+        <is>
+          <t>P3 (kW)</t>
+        </is>
+      </c>
+      <c r="R49" s="1" t="inlineStr">
+        <is>
+          <t>Q3 (kVAr)</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>671</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>1</v>
+      </c>
+      <c r="C50" t="n">
+        <v>4.16</v>
+      </c>
+      <c r="D50" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>delta</t>
+        </is>
+      </c>
+      <c r="F50" t="n">
+        <v>0</v>
+      </c>
+      <c r="G50" t="n">
+        <v>0</v>
+      </c>
+      <c r="H50" t="n">
+        <v>100</v>
+      </c>
+      <c r="I50" t="n">
+        <v>0</v>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>671_A</t>
+        </is>
+      </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>671_B</t>
+        </is>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>671_C</t>
+        </is>
+      </c>
+      <c r="M50" t="n">
+        <v>385</v>
+      </c>
+      <c r="N50" t="n">
+        <v>220</v>
+      </c>
+      <c r="O50" t="n">
+        <v>385</v>
+      </c>
+      <c r="P50" t="n">
+        <v>220</v>
+      </c>
+      <c r="Q50" t="n">
+        <v>385</v>
+      </c>
+      <c r="R50" t="n">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>pv_school</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>1</v>
+      </c>
+      <c r="C51" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="D51" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>wye</t>
+        </is>
+      </c>
+      <c r="F51" t="n">
+        <v>0</v>
+      </c>
+      <c r="G51" t="n">
+        <v>100</v>
+      </c>
+      <c r="H51" t="n">
+        <v>0</v>
+      </c>
+      <c r="I51" t="n">
+        <v>0</v>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>634_A</t>
+        </is>
+      </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>634_B</t>
+        </is>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>634_C</t>
+        </is>
+      </c>
+      <c r="M51" t="n">
+        <v>-80</v>
+      </c>
+      <c r="N51" t="n">
+        <v>-0</v>
+      </c>
+      <c r="O51" t="n">
+        <v>-80</v>
+      </c>
+      <c r="P51" t="n">
+        <v>-0</v>
+      </c>
+      <c r="Q51" t="n">
+        <v>-80</v>
+      </c>
+      <c r="R51" t="n">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>bat_school</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>1</v>
+      </c>
+      <c r="C52" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="D52" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>wye</t>
+        </is>
+      </c>
+      <c r="F52" t="n">
+        <v>0</v>
+      </c>
+      <c r="G52" t="n">
+        <v>100</v>
+      </c>
+      <c r="H52" t="n">
+        <v>0</v>
+      </c>
+      <c r="I52" t="n">
+        <v>0</v>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>634_A</t>
+        </is>
+      </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>634_B</t>
+        </is>
+      </c>
+      <c r="L52" t="inlineStr">
+        <is>
+          <t>634_C</t>
+        </is>
+      </c>
+      <c r="M52" t="n">
+        <v>33.33333333333334</v>
+      </c>
+      <c r="N52" t="n">
+        <v>-0</v>
+      </c>
+      <c r="O52" t="n">
+        <v>33.33333333333334</v>
+      </c>
+      <c r="P52" t="n">
+        <v>-0</v>
+      </c>
+      <c r="Q52" t="n">
+        <v>33.33333333333334</v>
+      </c>
+      <c r="R52" t="n">
+        <v>-0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
         <is>
           <t>End of ThreePhase ZIP Load</t>
         </is>
@@ -1183,7 +2162,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A11:N25"/>
+  <dimension ref="A11:N27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1274,157 +2253,233 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
+          <t>cap2</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>611_C</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>99.99999935999998</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
           <t>End of Single-Phase Shunt</t>
         </is>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
+    <row r="20">
+      <c r="A20" t="inlineStr">
         <is>
           <t>Two-Phase Shunt</t>
         </is>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="1" t="inlineStr">
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="B20" s="1" t="inlineStr">
+      <c r="B21" s="1" t="inlineStr">
         <is>
           <t>Status1</t>
         </is>
       </c>
-      <c r="C20" s="1" t="inlineStr">
+      <c r="C21" s="1" t="inlineStr">
         <is>
           <t>Status2</t>
         </is>
       </c>
-      <c r="D20" s="1" t="inlineStr">
+      <c r="D21" s="1" t="inlineStr">
         <is>
           <t>kV (ph-gr RMS)</t>
         </is>
       </c>
-      <c r="E20" s="1" t="inlineStr">
+      <c r="E21" s="1" t="inlineStr">
         <is>
           <t>Bus1</t>
         </is>
       </c>
-      <c r="F20" s="1" t="inlineStr">
+      <c r="F21" s="1" t="inlineStr">
         <is>
           <t>Bus2</t>
         </is>
       </c>
-      <c r="G20" s="1" t="inlineStr">
+      <c r="G21" s="1" t="inlineStr">
         <is>
           <t>P1 (kW)</t>
         </is>
       </c>
-      <c r="H20" s="1" t="inlineStr">
+      <c r="H21" s="1" t="inlineStr">
         <is>
           <t>Q1 (kVAr)</t>
         </is>
       </c>
-      <c r="I20" s="1" t="inlineStr">
+      <c r="I21" s="1" t="inlineStr">
         <is>
           <t>P2 (kW)</t>
         </is>
       </c>
-      <c r="J20" s="1" t="inlineStr">
+      <c r="J21" s="1" t="inlineStr">
         <is>
           <t>Q2 (kVAr)</t>
         </is>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
+    <row r="22">
+      <c r="A22" t="inlineStr">
         <is>
           <t>End of Two-Phase Shunt</t>
         </is>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
+    <row r="24">
+      <c r="A24" t="inlineStr">
         <is>
           <t>Three-Phase Shunt</t>
         </is>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="1" t="inlineStr">
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="B24" s="1" t="inlineStr">
+      <c r="B25" s="1" t="inlineStr">
         <is>
           <t>Status1</t>
         </is>
       </c>
-      <c r="C24" s="1" t="inlineStr">
+      <c r="C25" s="1" t="inlineStr">
         <is>
           <t>Status2</t>
         </is>
       </c>
-      <c r="D24" s="1" t="inlineStr">
+      <c r="D25" s="1" t="inlineStr">
         <is>
           <t>Status3</t>
         </is>
       </c>
-      <c r="E24" s="1" t="inlineStr">
+      <c r="E25" s="1" t="inlineStr">
         <is>
           <t>kV (ph-gr RMS)</t>
         </is>
       </c>
-      <c r="F24" s="1" t="inlineStr">
+      <c r="F25" s="1" t="inlineStr">
         <is>
           <t>Bus1</t>
         </is>
       </c>
-      <c r="G24" s="1" t="inlineStr">
+      <c r="G25" s="1" t="inlineStr">
         <is>
           <t>Bus2</t>
         </is>
       </c>
-      <c r="H24" s="1" t="inlineStr">
+      <c r="H25" s="1" t="inlineStr">
         <is>
           <t>Bus3</t>
         </is>
       </c>
-      <c r="I24" s="1" t="inlineStr">
+      <c r="I25" s="1" t="inlineStr">
         <is>
           <t>P1 (kW)</t>
         </is>
       </c>
-      <c r="J24" s="1" t="inlineStr">
+      <c r="J25" s="1" t="inlineStr">
         <is>
           <t>Q1 (kVAr)</t>
         </is>
       </c>
-      <c r="K24" s="1" t="inlineStr">
+      <c r="K25" s="1" t="inlineStr">
         <is>
           <t>P2 (kW)</t>
         </is>
       </c>
-      <c r="L24" s="1" t="inlineStr">
+      <c r="L25" s="1" t="inlineStr">
         <is>
           <t>Q2 (kVAr)</t>
         </is>
       </c>
-      <c r="M24" s="1" t="inlineStr">
+      <c r="M25" s="1" t="inlineStr">
         <is>
           <t>P3 (kW)</t>
         </is>
       </c>
-      <c r="N24" s="1" t="inlineStr">
+      <c r="N25" s="1" t="inlineStr">
         <is>
           <t>Q3 (kVAr)</t>
         </is>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>cap1</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>1</v>
+      </c>
+      <c r="C26" t="n">
+        <v>1</v>
+      </c>
+      <c r="D26" t="n">
+        <v>1</v>
+      </c>
+      <c r="E26" t="n">
+        <v>2.401777119828843</v>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>675_A</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>675_B</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>675_C</t>
+        </is>
+      </c>
+      <c r="I26" t="n">
+        <v>0</v>
+      </c>
+      <c r="J26" t="n">
+        <v>200.0000000682666</v>
+      </c>
+      <c r="K26" t="n">
+        <v>0</v>
+      </c>
+      <c r="L26" t="n">
+        <v>200.0000000682666</v>
+      </c>
+      <c r="M26" t="n">
+        <v>0</v>
+      </c>
+      <c r="N26" t="n">
+        <v>200.0000000682666</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
         <is>
           <t>End of Three-Phase Shunt</t>
         </is>
@@ -2467,7 +3522,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>632_B</t>
+          <t>632_C</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -2482,7 +3537,7 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -2493,7 +3548,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>632_C</t>
+          <t>632_A</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -2508,7 +3563,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -2519,7 +3574,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>632_A</t>
+          <t>632_B</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -2534,7 +3589,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -2545,7 +3600,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>633_B</t>
+          <t>633_C</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -2560,7 +3615,7 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -2571,7 +3626,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>633_C</t>
+          <t>633_A</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -2586,7 +3641,7 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -2597,7 +3652,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>633_A</t>
+          <t>633_B</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -2612,7 +3667,7 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -2623,7 +3678,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>634_B</t>
+          <t>634_C</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -2638,7 +3693,7 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -2649,7 +3704,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>634_C</t>
+          <t>634_A</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -2664,7 +3719,7 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -2675,7 +3730,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>634_A</t>
+          <t>634_B</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -2690,7 +3745,7 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -2701,7 +3756,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>645_B</t>
+          <t>645_C</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -2716,7 +3771,7 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -2727,7 +3782,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>645_C</t>
+          <t>645_B</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -2742,7 +3797,7 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -2753,7 +3808,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>646_B</t>
+          <t>646_C</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -2768,7 +3823,7 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
@@ -2779,7 +3834,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>646_C</t>
+          <t>646_B</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -2794,7 +3849,7 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -2805,7 +3860,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>650_B</t>
+          <t>650_C</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -2820,7 +3875,7 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -2831,7 +3886,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>650_C</t>
+          <t>650_A</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -2846,7 +3901,7 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -2857,7 +3912,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>650_A</t>
+          <t>650_B</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -2872,7 +3927,7 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
@@ -2909,7 +3964,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>670_B</t>
+          <t>670_C</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -2924,7 +3979,7 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -2935,7 +3990,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>670_C</t>
+          <t>670_A</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -2950,7 +4005,7 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
@@ -2961,7 +4016,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>670_A</t>
+          <t>670_B</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -2976,7 +4031,7 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
@@ -2987,7 +4042,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>671_B</t>
+          <t>671_C</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -3002,7 +4057,7 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
@@ -3013,7 +4068,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>671_C</t>
+          <t>671_A</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -3028,7 +4083,7 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
@@ -3039,7 +4094,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>671_A</t>
+          <t>671_B</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -3054,7 +4109,7 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -3065,7 +4120,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>675_B</t>
+          <t>675_C</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -3080,7 +4135,7 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
@@ -3091,7 +4146,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>675_C</t>
+          <t>675_A</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -3106,7 +4161,7 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
@@ -3117,7 +4172,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>675_A</t>
+          <t>675_B</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -3132,7 +4187,7 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
@@ -3143,7 +4198,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>680_B</t>
+          <t>680_C</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -3158,7 +4213,7 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
@@ -3169,7 +4224,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>680_C</t>
+          <t>680_A</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -3184,7 +4239,7 @@
         </is>
       </c>
       <c r="E30" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
@@ -3195,7 +4250,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>680_A</t>
+          <t>680_B</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -3210,7 +4265,7 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
@@ -3273,7 +4328,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>692_B</t>
+          <t>692_C</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -3288,7 +4343,7 @@
         </is>
       </c>
       <c r="E34" t="n">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
@@ -3299,7 +4354,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>692_C</t>
+          <t>692_A</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -3314,7 +4369,7 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
@@ -3325,7 +4380,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>692_A</t>
+          <t>692_B</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -3340,7 +4395,7 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
@@ -3351,7 +4406,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>brkr_B</t>
+          <t>brkr_C</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -3366,7 +4421,7 @@
         </is>
       </c>
       <c r="E37" t="n">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
@@ -3377,7 +4432,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>brkr_C</t>
+          <t>brkr_A</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -3392,7 +4447,7 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
@@ -3403,7 +4458,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>brkr_A</t>
+          <t>brkr_B</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -3418,7 +4473,7 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
@@ -3429,7 +4484,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>house_s2</t>
+          <t>house_s1</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -3444,7 +4499,7 @@
         </is>
       </c>
       <c r="E40" t="n">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
@@ -3455,7 +4510,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>house_s1</t>
+          <t>house_s2</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -3470,7 +4525,7 @@
         </is>
       </c>
       <c r="E41" t="n">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
@@ -3481,7 +4536,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>mid_B</t>
+          <t>mid_C</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -3496,7 +4551,7 @@
         </is>
       </c>
       <c r="E42" t="n">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
@@ -3507,7 +4562,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>mid_C</t>
+          <t>mid_A</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -3522,7 +4577,7 @@
         </is>
       </c>
       <c r="E43" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
@@ -3533,7 +4588,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>mid_A</t>
+          <t>mid_B</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -3548,7 +4603,7 @@
         </is>
       </c>
       <c r="E44" t="n">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
@@ -3559,7 +4614,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>rg60_B</t>
+          <t>rg60_C</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -3574,7 +4629,7 @@
         </is>
       </c>
       <c r="E45" t="n">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
@@ -3585,7 +4640,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>rg60_C</t>
+          <t>rg60_A</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -3600,7 +4655,7 @@
         </is>
       </c>
       <c r="E46" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
@@ -3611,7 +4666,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>rg60_A</t>
+          <t>rg60_B</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -3626,7 +4681,7 @@
         </is>
       </c>
       <c r="E47" t="n">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
@@ -3637,7 +4692,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>sourcebus_B</t>
+          <t>sourcebus_C</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -3652,7 +4707,7 @@
         </is>
       </c>
       <c r="E48" t="n">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
@@ -3663,7 +4718,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>sourcebus_C</t>
+          <t>sourcebus_A</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -3678,7 +4733,7 @@
         </is>
       </c>
       <c r="E49" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
@@ -3689,7 +4744,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>sourcebus_A</t>
+          <t>sourcebus_B</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -3704,7 +4759,7 @@
         </is>
       </c>
       <c r="E50" t="n">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
@@ -3741,7 +4796,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>xf1_B</t>
+          <t>xf1_C</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -3756,7 +4811,7 @@
         </is>
       </c>
       <c r="E52" t="n">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F52" t="inlineStr">
         <is>
@@ -3767,7 +4822,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>xf1_C</t>
+          <t>xf1_A</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -3782,7 +4837,7 @@
         </is>
       </c>
       <c r="E53" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F53" t="inlineStr">
         <is>
@@ -3793,7 +4848,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>xf1_A</t>
+          <t>xf1_B</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -3808,7 +4863,7 @@
         </is>
       </c>
       <c r="E54" t="n">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
writing lines from DistLinesCodeZ
</commit_message>
<xml_diff>
--- a/CPYDAR/ieee13x.xlsx
+++ b/CPYDAR/ieee13x.xlsx
@@ -2496,7 +2496,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A11:AA29"/>
+  <dimension ref="A11:AA40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2607,343 +2607,1169 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>End of Single-Phase Line</t>
-        </is>
+          <t>684611</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" t="n">
+        <v>91.44</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>tap_C</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>611_C</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>0.00082592659</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.00083729768</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>684652</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" t="n">
+        <v>243.84</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>684_A</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>652_A</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>0.00083419083</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.0003183906</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.055283335</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Two-Phase Line</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="B20" s="1" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
-      </c>
-      <c r="C20" s="1" t="inlineStr">
-        <is>
-          <t>Length</t>
-        </is>
-      </c>
-      <c r="D20" s="1" t="inlineStr">
-        <is>
-          <t>From1</t>
-        </is>
-      </c>
-      <c r="E20" s="1" t="inlineStr">
-        <is>
-          <t>From2</t>
-        </is>
-      </c>
-      <c r="F20" s="1" t="inlineStr">
-        <is>
-          <t>To1</t>
-        </is>
-      </c>
-      <c r="G20" s="1" t="inlineStr">
-        <is>
-          <t>To2</t>
-        </is>
-      </c>
-      <c r="H20" s="1" t="inlineStr">
-        <is>
-          <t>r11 (Ohm/length_unit)</t>
-        </is>
-      </c>
-      <c r="I20" s="1" t="inlineStr">
-        <is>
-          <t>x11 (Ohm/length_unit)</t>
-        </is>
-      </c>
-      <c r="J20" s="1" t="inlineStr">
-        <is>
-          <t>r21 (Ohm/length_unit)</t>
-        </is>
-      </c>
-      <c r="K20" s="1" t="inlineStr">
-        <is>
-          <t>x21 (Ohm/length_unit)</t>
-        </is>
-      </c>
-      <c r="L20" s="1" t="inlineStr">
-        <is>
-          <t>r22 (Ohm/length_unit)</t>
-        </is>
-      </c>
-      <c r="M20" s="1" t="inlineStr">
-        <is>
-          <t>x22 (Ohm/length_unit)</t>
-        </is>
-      </c>
-      <c r="N20" s="1" t="inlineStr">
-        <is>
-          <t>b11 (uS/length_unit)</t>
-        </is>
-      </c>
-      <c r="O20" s="1" t="inlineStr">
-        <is>
-          <t>b21 (uS/length_unit)</t>
-        </is>
-      </c>
-      <c r="P20" s="1" t="inlineStr">
-        <is>
-          <t>b22 (uS/length_unit)</t>
+          <t>End of Single-Phase Line</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>End of Two-Phase Line</t>
+          <t>Two-Phase Line</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B22" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="C22" s="1" t="inlineStr">
+        <is>
+          <t>Length</t>
+        </is>
+      </c>
+      <c r="D22" s="1" t="inlineStr">
+        <is>
+          <t>From1</t>
+        </is>
+      </c>
+      <c r="E22" s="1" t="inlineStr">
+        <is>
+          <t>From2</t>
+        </is>
+      </c>
+      <c r="F22" s="1" t="inlineStr">
+        <is>
+          <t>To1</t>
+        </is>
+      </c>
+      <c r="G22" s="1" t="inlineStr">
+        <is>
+          <t>To2</t>
+        </is>
+      </c>
+      <c r="H22" s="1" t="inlineStr">
+        <is>
+          <t>r11 (Ohm/length_unit)</t>
+        </is>
+      </c>
+      <c r="I22" s="1" t="inlineStr">
+        <is>
+          <t>x11 (Ohm/length_unit)</t>
+        </is>
+      </c>
+      <c r="J22" s="1" t="inlineStr">
+        <is>
+          <t>r21 (Ohm/length_unit)</t>
+        </is>
+      </c>
+      <c r="K22" s="1" t="inlineStr">
+        <is>
+          <t>x21 (Ohm/length_unit)</t>
+        </is>
+      </c>
+      <c r="L22" s="1" t="inlineStr">
+        <is>
+          <t>r22 (Ohm/length_unit)</t>
+        </is>
+      </c>
+      <c r="M22" s="1" t="inlineStr">
+        <is>
+          <t>x22 (Ohm/length_unit)</t>
+        </is>
+      </c>
+      <c r="N22" s="1" t="inlineStr">
+        <is>
+          <t>b11 (uS/length_unit)</t>
+        </is>
+      </c>
+      <c r="O22" s="1" t="inlineStr">
+        <is>
+          <t>b21 (uS/length_unit)</t>
+        </is>
+      </c>
+      <c r="P22" s="1" t="inlineStr">
+        <is>
+          <t>b22 (uS/length_unit)</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Three-Phase Line with Full Data</t>
-        </is>
+          <t>632645</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>1</v>
+      </c>
+      <c r="C23" t="n">
+        <v>152.4</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>632_C</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>632_B</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>645_C</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>645_B</t>
+        </is>
+      </c>
+      <c r="H23" t="n">
+        <v>0.00082257118</v>
+      </c>
+      <c r="I23" t="n">
+        <v>0.00084313857</v>
+      </c>
+      <c r="J23" t="n">
+        <v>0.00012837529</v>
+      </c>
+      <c r="K23" t="n">
+        <v>0.00028527151</v>
+      </c>
+      <c r="L23" t="n">
+        <v>0.00082605086</v>
+      </c>
+      <c r="M23" t="n">
+        <v>0.00083704913</v>
+      </c>
+      <c r="N23" t="n">
+        <v>0</v>
+      </c>
+      <c r="O23" t="n">
+        <v>0</v>
+      </c>
+      <c r="P23" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="1" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="B24" s="1" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
-      </c>
-      <c r="C24" s="1" t="inlineStr">
-        <is>
-          <t>Length</t>
-        </is>
-      </c>
-      <c r="D24" s="1" t="inlineStr">
-        <is>
-          <t>From1</t>
-        </is>
-      </c>
-      <c r="E24" s="1" t="inlineStr">
-        <is>
-          <t>From2</t>
-        </is>
-      </c>
-      <c r="F24" s="1" t="inlineStr">
-        <is>
-          <t>From3</t>
-        </is>
-      </c>
-      <c r="G24" s="1" t="inlineStr">
-        <is>
-          <t>To1</t>
-        </is>
-      </c>
-      <c r="H24" s="1" t="inlineStr">
-        <is>
-          <t>To2</t>
-        </is>
-      </c>
-      <c r="I24" s="1" t="inlineStr">
-        <is>
-          <t>To3</t>
-        </is>
-      </c>
-      <c r="J24" s="1" t="inlineStr">
-        <is>
-          <t>r11 (Ohm/length_unit)</t>
-        </is>
-      </c>
-      <c r="K24" s="1" t="inlineStr">
-        <is>
-          <t>x11 (Ohm/length_unit)</t>
-        </is>
-      </c>
-      <c r="L24" s="1" t="inlineStr">
-        <is>
-          <t>r21 (Ohm/length_unit)</t>
-        </is>
-      </c>
-      <c r="M24" s="1" t="inlineStr">
-        <is>
-          <t>x21 (Ohm/length_unit)</t>
-        </is>
-      </c>
-      <c r="N24" s="1" t="inlineStr">
-        <is>
-          <t>r22 (Ohm/length_unit)</t>
-        </is>
-      </c>
-      <c r="O24" s="1" t="inlineStr">
-        <is>
-          <t>x22 (Ohm/length_unit)</t>
-        </is>
-      </c>
-      <c r="P24" s="1" t="inlineStr">
-        <is>
-          <t>r31 (Ohm/length_unit)</t>
-        </is>
-      </c>
-      <c r="Q24" s="1" t="inlineStr">
-        <is>
-          <t>x31 (Ohm/length_unit)</t>
-        </is>
-      </c>
-      <c r="R24" s="1" t="inlineStr">
-        <is>
-          <t>r32 (Ohm/length_unit)</t>
-        </is>
-      </c>
-      <c r="S24" s="1" t="inlineStr">
-        <is>
-          <t>x32 (Ohm/length_unit)</t>
-        </is>
-      </c>
-      <c r="T24" s="1" t="inlineStr">
-        <is>
-          <t>r33 (Ohm/length_unit)</t>
-        </is>
-      </c>
-      <c r="U24" s="1" t="inlineStr">
-        <is>
-          <t>x33 (Ohm/length_unit)</t>
-        </is>
-      </c>
-      <c r="V24" s="1" t="inlineStr">
-        <is>
-          <t>b11 (uS/length_unit)</t>
-        </is>
-      </c>
-      <c r="W24" s="1" t="inlineStr">
-        <is>
-          <t>b21 (uS/length_unit)</t>
-        </is>
-      </c>
-      <c r="X24" s="1" t="inlineStr">
-        <is>
-          <t>b22 (uS/length_unit)</t>
-        </is>
-      </c>
-      <c r="Y24" s="1" t="inlineStr">
-        <is>
-          <t>b31 (uS/length_unit)</t>
-        </is>
-      </c>
-      <c r="Z24" s="1" t="inlineStr">
-        <is>
-          <t>b32 (uS/length_unit)</t>
-        </is>
-      </c>
-      <c r="AA24" s="1" t="inlineStr">
-        <is>
-          <t>b33 (uS/length_unit)</t>
-        </is>
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>645646</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>1</v>
+      </c>
+      <c r="C24" t="n">
+        <v>91.44</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>645_C</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>645_B</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>646_C</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>646_B</t>
+        </is>
+      </c>
+      <c r="H24" t="n">
+        <v>0.00082257118</v>
+      </c>
+      <c r="I24" t="n">
+        <v>0.00084313857</v>
+      </c>
+      <c r="J24" t="n">
+        <v>0.00012837529</v>
+      </c>
+      <c r="K24" t="n">
+        <v>0.00028527151</v>
+      </c>
+      <c r="L24" t="n">
+        <v>0.00082605086</v>
+      </c>
+      <c r="M24" t="n">
+        <v>0.00083704913</v>
+      </c>
+      <c r="N24" t="n">
+        <v>0</v>
+      </c>
+      <c r="O24" t="n">
+        <v>0</v>
+      </c>
+      <c r="P24" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
+          <t>671684</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>1</v>
+      </c>
+      <c r="C25" t="n">
+        <v>91.44</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>671_A</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>671_C</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>684_A</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>684_C</t>
+        </is>
+      </c>
+      <c r="H25" t="n">
+        <v>0.00082257118</v>
+      </c>
+      <c r="I25" t="n">
+        <v>0.00084313857</v>
+      </c>
+      <c r="J25" t="n">
+        <v>0.00012837529</v>
+      </c>
+      <c r="K25" t="n">
+        <v>0.00028527151</v>
+      </c>
+      <c r="L25" t="n">
+        <v>0.00082605086</v>
+      </c>
+      <c r="M25" t="n">
+        <v>0.00083704913</v>
+      </c>
+      <c r="N25" t="n">
+        <v>0</v>
+      </c>
+      <c r="O25" t="n">
+        <v>0</v>
+      </c>
+      <c r="P25" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>End of Two-Phase Line</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Three-Phase Line with Full Data</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B29" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="C29" s="1" t="inlineStr">
+        <is>
+          <t>Length</t>
+        </is>
+      </c>
+      <c r="D29" s="1" t="inlineStr">
+        <is>
+          <t>From1</t>
+        </is>
+      </c>
+      <c r="E29" s="1" t="inlineStr">
+        <is>
+          <t>From2</t>
+        </is>
+      </c>
+      <c r="F29" s="1" t="inlineStr">
+        <is>
+          <t>From3</t>
+        </is>
+      </c>
+      <c r="G29" s="1" t="inlineStr">
+        <is>
+          <t>To1</t>
+        </is>
+      </c>
+      <c r="H29" s="1" t="inlineStr">
+        <is>
+          <t>To2</t>
+        </is>
+      </c>
+      <c r="I29" s="1" t="inlineStr">
+        <is>
+          <t>To3</t>
+        </is>
+      </c>
+      <c r="J29" s="1" t="inlineStr">
+        <is>
+          <t>r11 (Ohm/length_unit)</t>
+        </is>
+      </c>
+      <c r="K29" s="1" t="inlineStr">
+        <is>
+          <t>x11 (Ohm/length_unit)</t>
+        </is>
+      </c>
+      <c r="L29" s="1" t="inlineStr">
+        <is>
+          <t>r21 (Ohm/length_unit)</t>
+        </is>
+      </c>
+      <c r="M29" s="1" t="inlineStr">
+        <is>
+          <t>x21 (Ohm/length_unit)</t>
+        </is>
+      </c>
+      <c r="N29" s="1" t="inlineStr">
+        <is>
+          <t>r22 (Ohm/length_unit)</t>
+        </is>
+      </c>
+      <c r="O29" s="1" t="inlineStr">
+        <is>
+          <t>x22 (Ohm/length_unit)</t>
+        </is>
+      </c>
+      <c r="P29" s="1" t="inlineStr">
+        <is>
+          <t>r31 (Ohm/length_unit)</t>
+        </is>
+      </c>
+      <c r="Q29" s="1" t="inlineStr">
+        <is>
+          <t>x31 (Ohm/length_unit)</t>
+        </is>
+      </c>
+      <c r="R29" s="1" t="inlineStr">
+        <is>
+          <t>r32 (Ohm/length_unit)</t>
+        </is>
+      </c>
+      <c r="S29" s="1" t="inlineStr">
+        <is>
+          <t>x32 (Ohm/length_unit)</t>
+        </is>
+      </c>
+      <c r="T29" s="1" t="inlineStr">
+        <is>
+          <t>r33 (Ohm/length_unit)</t>
+        </is>
+      </c>
+      <c r="U29" s="1" t="inlineStr">
+        <is>
+          <t>x33 (Ohm/length_unit)</t>
+        </is>
+      </c>
+      <c r="V29" s="1" t="inlineStr">
+        <is>
+          <t>b11 (uS/length_unit)</t>
+        </is>
+      </c>
+      <c r="W29" s="1" t="inlineStr">
+        <is>
+          <t>b21 (uS/length_unit)</t>
+        </is>
+      </c>
+      <c r="X29" s="1" t="inlineStr">
+        <is>
+          <t>b22 (uS/length_unit)</t>
+        </is>
+      </c>
+      <c r="Y29" s="1" t="inlineStr">
+        <is>
+          <t>b31 (uS/length_unit)</t>
+        </is>
+      </c>
+      <c r="Z29" s="1" t="inlineStr">
+        <is>
+          <t>b32 (uS/length_unit)</t>
+        </is>
+      </c>
+      <c r="AA29" s="1" t="inlineStr">
+        <is>
+          <t>b33 (uS/length_unit)</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>632633</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>1</v>
+      </c>
+      <c r="C30" t="n">
+        <v>152.4</v>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>632_A</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>632_B</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>632_C</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>633_A</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>633_B</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>633_C</t>
+        </is>
+      </c>
+      <c r="J30" t="n">
+        <v>0.00046764396</v>
+      </c>
+      <c r="K30" t="n">
+        <v>0.00073408793</v>
+      </c>
+      <c r="L30" t="n">
+        <v>9.5380478e-05</v>
+      </c>
+      <c r="M30" t="n">
+        <v>0.00023916577</v>
+      </c>
+      <c r="N30" t="n">
+        <v>0.00046447497</v>
+      </c>
+      <c r="O30" t="n">
+        <v>0.0007445891</v>
+      </c>
+      <c r="P30" t="n">
+        <v>9.6933906e-05</v>
+      </c>
+      <c r="Q30" t="n">
+        <v>0.00031174193</v>
+      </c>
+      <c r="R30" t="n">
+        <v>9.8176648e-05</v>
+      </c>
+      <c r="S30" t="n">
+        <v>0.00026321284</v>
+      </c>
+      <c r="T30" t="n">
+        <v>0.00046205162</v>
+      </c>
+      <c r="U30" t="n">
+        <v>0.00075260479</v>
+      </c>
+      <c r="V30" t="n">
+        <v>0</v>
+      </c>
+      <c r="W30" t="n">
+        <v>0</v>
+      </c>
+      <c r="X30" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y30" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA30" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>632670</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>1</v>
+      </c>
+      <c r="C31" t="n">
+        <v>203.3016</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>mid_A</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>mid_B</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>mid_C</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>670_A</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>670_B</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>670_C</t>
+        </is>
+      </c>
+      <c r="J31" t="n">
+        <v>0.00021530512</v>
+      </c>
+      <c r="K31" t="n">
+        <v>0.00063249374</v>
+      </c>
+      <c r="L31" t="n">
+        <v>9.5380478e-05</v>
+      </c>
+      <c r="M31" t="n">
+        <v>0.00023916577</v>
+      </c>
+      <c r="N31" t="n">
+        <v>0.00020971278</v>
+      </c>
+      <c r="O31" t="n">
+        <v>0.00065107274</v>
+      </c>
+      <c r="P31" t="n">
+        <v>9.8176648e-05</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>0.00026321284</v>
+      </c>
+      <c r="R31" t="n">
+        <v>9.6933906e-05</v>
+      </c>
+      <c r="S31" t="n">
+        <v>0.00031174193</v>
+      </c>
+      <c r="T31" t="n">
+        <v>0.00021213613</v>
+      </c>
+      <c r="U31" t="n">
+        <v>0.00064299491</v>
+      </c>
+      <c r="V31" t="n">
+        <v>0</v>
+      </c>
+      <c r="W31" t="n">
+        <v>0</v>
+      </c>
+      <c r="X31" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y31" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA31" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>650632</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>1</v>
+      </c>
+      <c r="C32" t="n">
+        <v>609.6</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>rg60_A</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>rg60_B</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>rg60_C</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>632_A</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>632_B</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>632_C</t>
+        </is>
+      </c>
+      <c r="J32" t="n">
+        <v>0.00021530512</v>
+      </c>
+      <c r="K32" t="n">
+        <v>0.00063249374</v>
+      </c>
+      <c r="L32" t="n">
+        <v>9.5380478e-05</v>
+      </c>
+      <c r="M32" t="n">
+        <v>0.00023916577</v>
+      </c>
+      <c r="N32" t="n">
+        <v>0.00020971278</v>
+      </c>
+      <c r="O32" t="n">
+        <v>0.00065107274</v>
+      </c>
+      <c r="P32" t="n">
+        <v>9.8176648e-05</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>0.00026321284</v>
+      </c>
+      <c r="R32" t="n">
+        <v>9.6933906e-05</v>
+      </c>
+      <c r="S32" t="n">
+        <v>0.00031174193</v>
+      </c>
+      <c r="T32" t="n">
+        <v>0.00021213613</v>
+      </c>
+      <c r="U32" t="n">
+        <v>0.00064299491</v>
+      </c>
+      <c r="V32" t="n">
+        <v>0</v>
+      </c>
+      <c r="W32" t="n">
+        <v>0</v>
+      </c>
+      <c r="X32" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y32" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA32" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>670671</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>1</v>
+      </c>
+      <c r="C33" t="n">
+        <v>406.2984</v>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>670_A</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>670_B</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>670_C</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>671_A</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>671_B</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>671_C</t>
+        </is>
+      </c>
+      <c r="J33" t="n">
+        <v>0.00021530512</v>
+      </c>
+      <c r="K33" t="n">
+        <v>0.00063249374</v>
+      </c>
+      <c r="L33" t="n">
+        <v>9.5380478e-05</v>
+      </c>
+      <c r="M33" t="n">
+        <v>0.00023916577</v>
+      </c>
+      <c r="N33" t="n">
+        <v>0.00020971278</v>
+      </c>
+      <c r="O33" t="n">
+        <v>0.00065107274</v>
+      </c>
+      <c r="P33" t="n">
+        <v>9.8176648e-05</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>0.00026321284</v>
+      </c>
+      <c r="R33" t="n">
+        <v>9.6933906e-05</v>
+      </c>
+      <c r="S33" t="n">
+        <v>0.00031174193</v>
+      </c>
+      <c r="T33" t="n">
+        <v>0.00021213613</v>
+      </c>
+      <c r="U33" t="n">
+        <v>0.00064299491</v>
+      </c>
+      <c r="V33" t="n">
+        <v>0</v>
+      </c>
+      <c r="W33" t="n">
+        <v>0</v>
+      </c>
+      <c r="X33" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y33" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>671680</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>1</v>
+      </c>
+      <c r="C34" t="n">
+        <v>304.8</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>671_A</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>671_B</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>671_C</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>680_A</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>680_B</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>680_C</t>
+        </is>
+      </c>
+      <c r="J34" t="n">
+        <v>0.00021530512</v>
+      </c>
+      <c r="K34" t="n">
+        <v>0.00063249374</v>
+      </c>
+      <c r="L34" t="n">
+        <v>9.5380478e-05</v>
+      </c>
+      <c r="M34" t="n">
+        <v>0.00023916577</v>
+      </c>
+      <c r="N34" t="n">
+        <v>0.00020971278</v>
+      </c>
+      <c r="O34" t="n">
+        <v>0.00065107274</v>
+      </c>
+      <c r="P34" t="n">
+        <v>9.8176648e-05</v>
+      </c>
+      <c r="Q34" t="n">
+        <v>0.00026321284</v>
+      </c>
+      <c r="R34" t="n">
+        <v>9.6933906e-05</v>
+      </c>
+      <c r="S34" t="n">
+        <v>0.00031174193</v>
+      </c>
+      <c r="T34" t="n">
+        <v>0.00021213613</v>
+      </c>
+      <c r="U34" t="n">
+        <v>0.00064299491</v>
+      </c>
+      <c r="V34" t="n">
+        <v>0</v>
+      </c>
+      <c r="W34" t="n">
+        <v>0</v>
+      </c>
+      <c r="X34" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y34" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA34" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>692675</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>1</v>
+      </c>
+      <c r="C35" t="n">
+        <v>152.4</v>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>692_A</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>692_B</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>692_C</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>675_A</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>675_B</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>675_C</t>
+        </is>
+      </c>
+      <c r="J35" t="n">
+        <v>0.0004919526200000001</v>
+      </c>
+      <c r="K35" t="n">
+        <v>0.0002723793</v>
+      </c>
+      <c r="L35" t="n">
+        <v>0.00019789181</v>
+      </c>
+      <c r="M35" t="n">
+        <v>1.7201916e-05</v>
+      </c>
+      <c r="N35" t="n">
+        <v>0.00048569417</v>
+      </c>
+      <c r="O35" t="n">
+        <v>0.00024649609</v>
+      </c>
+      <c r="P35" t="n">
+        <v>0.00017612766</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>-1.1445906e-05</v>
+      </c>
+      <c r="R35" t="n">
+        <v>0.00019789181</v>
+      </c>
+      <c r="S35" t="n">
+        <v>1.7201916e-05</v>
+      </c>
+      <c r="T35" t="n">
+        <v>0.0004919526200000001</v>
+      </c>
+      <c r="U35" t="n">
+        <v>0.0002723793</v>
+      </c>
+      <c r="V35" t="n">
+        <v>0.08994036399999999</v>
+      </c>
+      <c r="W35" t="n">
+        <v>0</v>
+      </c>
+      <c r="X35" t="n">
+        <v>0.08994036399999999</v>
+      </c>
+      <c r="Y35" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA35" t="n">
+        <v>0.08994036399999999</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
           <t>End of Three-Phase Line with Full Data</t>
         </is>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
+    <row r="38">
+      <c r="A38" t="inlineStr">
         <is>
           <t>Three-Phase Line with Sequential Data</t>
         </is>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" s="1" t="inlineStr">
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
         <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="B28" s="1" t="inlineStr">
+      <c r="B39" s="1" t="inlineStr">
         <is>
           <t>Status</t>
         </is>
       </c>
-      <c r="C28" s="1" t="inlineStr">
+      <c r="C39" s="1" t="inlineStr">
         <is>
           <t>Length</t>
         </is>
       </c>
-      <c r="D28" s="1" t="inlineStr">
+      <c r="D39" s="1" t="inlineStr">
         <is>
           <t>From1</t>
         </is>
       </c>
-      <c r="E28" s="1" t="inlineStr">
+      <c r="E39" s="1" t="inlineStr">
         <is>
           <t>From2</t>
         </is>
       </c>
-      <c r="F28" s="1" t="inlineStr">
+      <c r="F39" s="1" t="inlineStr">
         <is>
           <t>From3</t>
         </is>
       </c>
-      <c r="G28" s="1" t="inlineStr">
+      <c r="G39" s="1" t="inlineStr">
         <is>
           <t>To1</t>
         </is>
       </c>
-      <c r="H28" s="1" t="inlineStr">
+      <c r="H39" s="1" t="inlineStr">
         <is>
           <t>To2</t>
         </is>
       </c>
-      <c r="I28" s="1" t="inlineStr">
+      <c r="I39" s="1" t="inlineStr">
         <is>
           <t>To3</t>
         </is>
       </c>
-      <c r="J28" s="1" t="inlineStr">
+      <c r="J39" s="1" t="inlineStr">
         <is>
           <t>R0 (Ohm/length_unit)</t>
         </is>
       </c>
-      <c r="K28" s="1" t="inlineStr">
+      <c r="K39" s="1" t="inlineStr">
         <is>
           <t>X0 (Ohm/length_unit)</t>
         </is>
       </c>
-      <c r="L28" s="1" t="inlineStr">
+      <c r="L39" s="1" t="inlineStr">
         <is>
           <t>R1 (Ohm/length_unit)</t>
         </is>
       </c>
-      <c r="M28" s="1" t="inlineStr">
+      <c r="M39" s="1" t="inlineStr">
         <is>
           <t>X1 (Ohm/length_unit)</t>
         </is>
       </c>
-      <c r="N28" s="1" t="inlineStr">
+      <c r="N39" s="1" t="inlineStr">
         <is>
           <t>B0 (uS/length_unit)</t>
         </is>
       </c>
-      <c r="O28" s="1" t="inlineStr">
+      <c r="O39" s="1" t="inlineStr">
         <is>
           <t>B1 (uS/length_unit)</t>
         </is>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
+    <row r="40">
+      <c r="A40" t="inlineStr">
         <is>
           <t>End of Three-Phase Line with Sequential Data</t>
         </is>
@@ -4484,7 +5310,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>house_s1</t>
+          <t>house_s2</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -4499,7 +5325,7 @@
         </is>
       </c>
       <c r="E40" t="n">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
@@ -4510,7 +5336,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>house_s2</t>
+          <t>house_s1</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -4525,7 +5351,7 @@
         </is>
       </c>
       <c r="E41" t="n">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
parsing 2W and 3W positive-sequence transformers, but they cannot be mixed in with multi-phase networks
</commit_message>
<xml_diff>
--- a/CPYDAR/ieee13x.xlsx
+++ b/CPYDAR/ieee13x.xlsx
@@ -3786,7 +3786,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A11:AA25"/>
+  <dimension ref="A11:AA27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3861,408 +3861,490 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>End of Positive-Sequence 2W Transformer</t>
-        </is>
+          <t>sub</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>sourcebus</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>650</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>1e-05</v>
+      </c>
+      <c r="F13" t="n">
+        <v>8.000000000000001e-05</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>1</v>
+      </c>
+      <c r="J13" t="n">
+        <v>1</v>
+      </c>
+      <c r="K13" t="n">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>xfm1</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>xf1</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>634</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>0.011</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>1</v>
+      </c>
+      <c r="J14" t="n">
+        <v>1</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Positive-Sequence 3W Transformer</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="B16" s="1" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
-      </c>
-      <c r="C16" s="1" t="inlineStr">
-        <is>
-          <t>Bus1</t>
-        </is>
-      </c>
-      <c r="D16" s="1" t="inlineStr">
-        <is>
-          <t>Bus2</t>
-        </is>
-      </c>
-      <c r="E16" s="1" t="inlineStr">
-        <is>
-          <t>Bus3</t>
-        </is>
-      </c>
-      <c r="F16" s="1" t="inlineStr">
-        <is>
-          <t>R_12 (pu)</t>
-        </is>
-      </c>
-      <c r="G16" s="1" t="inlineStr">
-        <is>
-          <t>Xl_12 (pu)</t>
-        </is>
-      </c>
-      <c r="H16" s="1" t="inlineStr">
-        <is>
-          <t>R_23 (pu)</t>
-        </is>
-      </c>
-      <c r="I16" s="1" t="inlineStr">
-        <is>
-          <t>Xl_23 (pu)</t>
-        </is>
-      </c>
-      <c r="J16" s="1" t="inlineStr">
-        <is>
-          <t>R_31 (pu)</t>
-        </is>
-      </c>
-      <c r="K16" s="1" t="inlineStr">
-        <is>
-          <t>Xl_31 (pu)</t>
-        </is>
-      </c>
-      <c r="L16" s="1" t="inlineStr">
-        <is>
-          <t>Gmag (pu)</t>
-        </is>
-      </c>
-      <c r="M16" s="1" t="inlineStr">
-        <is>
-          <t>Bmag (pu)</t>
-        </is>
-      </c>
-      <c r="N16" s="1" t="inlineStr">
-        <is>
-          <t>Ratio W1 (pu)</t>
-        </is>
-      </c>
-      <c r="O16" s="1" t="inlineStr">
-        <is>
-          <t>Ratio W2 (pu)</t>
-        </is>
-      </c>
-      <c r="P16" s="1" t="inlineStr">
-        <is>
-          <t>Ratio W3 (pu)</t>
-        </is>
-      </c>
-      <c r="Q16" s="1" t="inlineStr">
-        <is>
-          <t>Phase Shift W1 (deg)</t>
-        </is>
-      </c>
-      <c r="R16" s="1" t="inlineStr">
-        <is>
-          <t>Phase Shift W2 (deg)</t>
-        </is>
-      </c>
-      <c r="S16" s="1" t="inlineStr">
-        <is>
-          <t>Phase Shift W3 (deg)</t>
+          <t>End of Positive-Sequence 2W Transformer</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>End of Positive-Sequence 3W Transformer</t>
+          <t>Positive-Sequence 3W Transformer</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B18" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="C18" s="1" t="inlineStr">
+        <is>
+          <t>Bus1</t>
+        </is>
+      </c>
+      <c r="D18" s="1" t="inlineStr">
+        <is>
+          <t>Bus2</t>
+        </is>
+      </c>
+      <c r="E18" s="1" t="inlineStr">
+        <is>
+          <t>Bus3</t>
+        </is>
+      </c>
+      <c r="F18" s="1" t="inlineStr">
+        <is>
+          <t>R_12 (pu)</t>
+        </is>
+      </c>
+      <c r="G18" s="1" t="inlineStr">
+        <is>
+          <t>Xl_12 (pu)</t>
+        </is>
+      </c>
+      <c r="H18" s="1" t="inlineStr">
+        <is>
+          <t>R_23 (pu)</t>
+        </is>
+      </c>
+      <c r="I18" s="1" t="inlineStr">
+        <is>
+          <t>Xl_23 (pu)</t>
+        </is>
+      </c>
+      <c r="J18" s="1" t="inlineStr">
+        <is>
+          <t>R_31 (pu)</t>
+        </is>
+      </c>
+      <c r="K18" s="1" t="inlineStr">
+        <is>
+          <t>Xl_31 (pu)</t>
+        </is>
+      </c>
+      <c r="L18" s="1" t="inlineStr">
+        <is>
+          <t>Gmag (pu)</t>
+        </is>
+      </c>
+      <c r="M18" s="1" t="inlineStr">
+        <is>
+          <t>Bmag (pu)</t>
+        </is>
+      </c>
+      <c r="N18" s="1" t="inlineStr">
+        <is>
+          <t>Ratio W1 (pu)</t>
+        </is>
+      </c>
+      <c r="O18" s="1" t="inlineStr">
+        <is>
+          <t>Ratio W2 (pu)</t>
+        </is>
+      </c>
+      <c r="P18" s="1" t="inlineStr">
+        <is>
+          <t>Ratio W3 (pu)</t>
+        </is>
+      </c>
+      <c r="Q18" s="1" t="inlineStr">
+        <is>
+          <t>Phase Shift W1 (deg)</t>
+        </is>
+      </c>
+      <c r="R18" s="1" t="inlineStr">
+        <is>
+          <t>Phase Shift W2 (deg)</t>
+        </is>
+      </c>
+      <c r="S18" s="1" t="inlineStr">
+        <is>
+          <t>Phase Shift W3 (deg)</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Multiphase 2W Transformer</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="1" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="B20" s="1" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
-      </c>
-      <c r="C20" s="1" t="inlineStr">
-        <is>
-          <t>Number of phases</t>
-        </is>
-      </c>
-      <c r="D20" s="1" t="inlineStr">
-        <is>
-          <t>Bus1_A</t>
-        </is>
-      </c>
-      <c r="E20" s="1" t="inlineStr">
-        <is>
-          <t>Bus1_B</t>
-        </is>
-      </c>
-      <c r="F20" s="1" t="inlineStr">
-        <is>
-          <t>Bus1_C</t>
-        </is>
-      </c>
-      <c r="G20" s="1" t="inlineStr">
-        <is>
-          <t>V1 (kV)</t>
-        </is>
-      </c>
-      <c r="H20" s="1" t="inlineStr">
-        <is>
-          <t>S_base1 (kVA)</t>
-        </is>
-      </c>
-      <c r="I20" s="1" t="inlineStr">
-        <is>
-          <t>Conn. type1</t>
-        </is>
-      </c>
-      <c r="J20" s="1" t="inlineStr">
-        <is>
-          <t>Bus2_A</t>
-        </is>
-      </c>
-      <c r="K20" s="1" t="inlineStr">
-        <is>
-          <t>Bus2_B</t>
-        </is>
-      </c>
-      <c r="L20" s="1" t="inlineStr">
-        <is>
-          <t>Bus2_C</t>
-        </is>
-      </c>
-      <c r="M20" s="1" t="inlineStr">
-        <is>
-          <t>V2 (kV)</t>
-        </is>
-      </c>
-      <c r="N20" s="1" t="inlineStr">
-        <is>
-          <t>S_base2 (kVA)</t>
-        </is>
-      </c>
-      <c r="O20" s="1" t="inlineStr">
-        <is>
-          <t>Conn. type2</t>
-        </is>
-      </c>
-      <c r="P20" s="1" t="inlineStr">
-        <is>
-          <t>Tap 1</t>
-        </is>
-      </c>
-      <c r="Q20" s="1" t="inlineStr">
-        <is>
-          <t>Tap 2</t>
-        </is>
-      </c>
-      <c r="R20" s="1" t="inlineStr">
-        <is>
-          <t>Tap 3</t>
-        </is>
-      </c>
-      <c r="S20" s="1" t="inlineStr">
-        <is>
-          <t>Lowest Tap</t>
-        </is>
-      </c>
-      <c r="T20" s="1" t="inlineStr">
-        <is>
-          <t>Highest Tap</t>
-        </is>
-      </c>
-      <c r="U20" s="1" t="inlineStr">
-        <is>
-          <t>Min Range (%)</t>
-        </is>
-      </c>
-      <c r="V20" s="1" t="inlineStr">
-        <is>
-          <t>Max Range (%)</t>
-        </is>
-      </c>
-      <c r="W20" s="1" t="inlineStr">
-        <is>
-          <t>X (pu)</t>
-        </is>
-      </c>
-      <c r="X20" s="1" t="inlineStr">
-        <is>
-          <t>RW1 (pu)</t>
-        </is>
-      </c>
-      <c r="Y20" s="1" t="inlineStr">
-        <is>
-          <t>RW2</t>
+          <t>End of Positive-Sequence 3W Transformer</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>End of Multiphase 2W Transformer</t>
+          <t>Multiphase 2W Transformer</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B22" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="C22" s="1" t="inlineStr">
+        <is>
+          <t>Number of phases</t>
+        </is>
+      </c>
+      <c r="D22" s="1" t="inlineStr">
+        <is>
+          <t>Bus1_A</t>
+        </is>
+      </c>
+      <c r="E22" s="1" t="inlineStr">
+        <is>
+          <t>Bus1_B</t>
+        </is>
+      </c>
+      <c r="F22" s="1" t="inlineStr">
+        <is>
+          <t>Bus1_C</t>
+        </is>
+      </c>
+      <c r="G22" s="1" t="inlineStr">
+        <is>
+          <t>V1 (kV)</t>
+        </is>
+      </c>
+      <c r="H22" s="1" t="inlineStr">
+        <is>
+          <t>S_base1 (kVA)</t>
+        </is>
+      </c>
+      <c r="I22" s="1" t="inlineStr">
+        <is>
+          <t>Conn. type1</t>
+        </is>
+      </c>
+      <c r="J22" s="1" t="inlineStr">
+        <is>
+          <t>Bus2_A</t>
+        </is>
+      </c>
+      <c r="K22" s="1" t="inlineStr">
+        <is>
+          <t>Bus2_B</t>
+        </is>
+      </c>
+      <c r="L22" s="1" t="inlineStr">
+        <is>
+          <t>Bus2_C</t>
+        </is>
+      </c>
+      <c r="M22" s="1" t="inlineStr">
+        <is>
+          <t>V2 (kV)</t>
+        </is>
+      </c>
+      <c r="N22" s="1" t="inlineStr">
+        <is>
+          <t>S_base2 (kVA)</t>
+        </is>
+      </c>
+      <c r="O22" s="1" t="inlineStr">
+        <is>
+          <t>Conn. type2</t>
+        </is>
+      </c>
+      <c r="P22" s="1" t="inlineStr">
+        <is>
+          <t>Tap 1</t>
+        </is>
+      </c>
+      <c r="Q22" s="1" t="inlineStr">
+        <is>
+          <t>Tap 2</t>
+        </is>
+      </c>
+      <c r="R22" s="1" t="inlineStr">
+        <is>
+          <t>Tap 3</t>
+        </is>
+      </c>
+      <c r="S22" s="1" t="inlineStr">
+        <is>
+          <t>Lowest Tap</t>
+        </is>
+      </c>
+      <c r="T22" s="1" t="inlineStr">
+        <is>
+          <t>Highest Tap</t>
+        </is>
+      </c>
+      <c r="U22" s="1" t="inlineStr">
+        <is>
+          <t>Min Range (%)</t>
+        </is>
+      </c>
+      <c r="V22" s="1" t="inlineStr">
+        <is>
+          <t>Max Range (%)</t>
+        </is>
+      </c>
+      <c r="W22" s="1" t="inlineStr">
+        <is>
+          <t>X (pu)</t>
+        </is>
+      </c>
+      <c r="X22" s="1" t="inlineStr">
+        <is>
+          <t>RW1 (pu)</t>
+        </is>
+      </c>
+      <c r="Y22" s="1" t="inlineStr">
+        <is>
+          <t>RW2</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Multiphase 2W Transformer with Mutual Impedance</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="B24" s="1" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
-      </c>
-      <c r="C24" s="1" t="inlineStr">
-        <is>
-          <t>Number of phases</t>
-        </is>
-      </c>
-      <c r="D24" s="1" t="inlineStr">
-        <is>
-          <t>Bus1_A</t>
-        </is>
-      </c>
-      <c r="E24" s="1" t="inlineStr">
-        <is>
-          <t>Bus1_B</t>
-        </is>
-      </c>
-      <c r="F24" s="1" t="inlineStr">
-        <is>
-          <t>Bus1_C</t>
-        </is>
-      </c>
-      <c r="G24" s="1" t="inlineStr">
-        <is>
-          <t>V1 (kV)</t>
-        </is>
-      </c>
-      <c r="H24" s="1" t="inlineStr">
-        <is>
-          <t>S_base1 (kVA)</t>
-        </is>
-      </c>
-      <c r="I24" s="1" t="inlineStr">
-        <is>
-          <t>Conn. type1</t>
-        </is>
-      </c>
-      <c r="J24" s="1" t="inlineStr">
-        <is>
-          <t>Bus2_A</t>
-        </is>
-      </c>
-      <c r="K24" s="1" t="inlineStr">
-        <is>
-          <t>Bus2_B</t>
-        </is>
-      </c>
-      <c r="L24" s="1" t="inlineStr">
-        <is>
-          <t>Bus2_C</t>
-        </is>
-      </c>
-      <c r="M24" s="1" t="inlineStr">
-        <is>
-          <t>V2 (kV)</t>
-        </is>
-      </c>
-      <c r="N24" s="1" t="inlineStr">
-        <is>
-          <t>S_base2 (kVA)</t>
-        </is>
-      </c>
-      <c r="O24" s="1" t="inlineStr">
-        <is>
-          <t>Conn. type2</t>
-        </is>
-      </c>
-      <c r="P24" s="1" t="inlineStr">
-        <is>
-          <t>Tap 1</t>
-        </is>
-      </c>
-      <c r="Q24" s="1" t="inlineStr">
-        <is>
-          <t>Tap 2</t>
-        </is>
-      </c>
-      <c r="R24" s="1" t="inlineStr">
-        <is>
-          <t>Tap 3</t>
-        </is>
-      </c>
-      <c r="S24" s="1" t="inlineStr">
-        <is>
-          <t>Lowest Tap</t>
-        </is>
-      </c>
-      <c r="T24" s="1" t="inlineStr">
-        <is>
-          <t>Highest Tap</t>
-        </is>
-      </c>
-      <c r="U24" s="1" t="inlineStr">
-        <is>
-          <t>Min Range (%)</t>
-        </is>
-      </c>
-      <c r="V24" s="1" t="inlineStr">
-        <is>
-          <t>Max Range (%)</t>
-        </is>
-      </c>
-      <c r="W24" s="1" t="inlineStr">
-        <is>
-          <t>Z0 leakage (pu)</t>
-        </is>
-      </c>
-      <c r="X24" s="1" t="inlineStr">
-        <is>
-          <t>Z1 leakage (pu)</t>
-        </is>
-      </c>
-      <c r="Y24" s="1" t="inlineStr">
-        <is>
-          <t>X0/R0</t>
-        </is>
-      </c>
-      <c r="Z24" s="1" t="inlineStr">
-        <is>
-          <t>X1/R1</t>
-        </is>
-      </c>
-      <c r="AA24" s="1" t="inlineStr">
-        <is>
-          <t>No Load Loss (kW)</t>
+          <t>End of Multiphase 2W Transformer</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
+        <is>
+          <t>Multiphase 2W Transformer with Mutual Impedance</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B26" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="C26" s="1" t="inlineStr">
+        <is>
+          <t>Number of phases</t>
+        </is>
+      </c>
+      <c r="D26" s="1" t="inlineStr">
+        <is>
+          <t>Bus1_A</t>
+        </is>
+      </c>
+      <c r="E26" s="1" t="inlineStr">
+        <is>
+          <t>Bus1_B</t>
+        </is>
+      </c>
+      <c r="F26" s="1" t="inlineStr">
+        <is>
+          <t>Bus1_C</t>
+        </is>
+      </c>
+      <c r="G26" s="1" t="inlineStr">
+        <is>
+          <t>V1 (kV)</t>
+        </is>
+      </c>
+      <c r="H26" s="1" t="inlineStr">
+        <is>
+          <t>S_base1 (kVA)</t>
+        </is>
+      </c>
+      <c r="I26" s="1" t="inlineStr">
+        <is>
+          <t>Conn. type1</t>
+        </is>
+      </c>
+      <c r="J26" s="1" t="inlineStr">
+        <is>
+          <t>Bus2_A</t>
+        </is>
+      </c>
+      <c r="K26" s="1" t="inlineStr">
+        <is>
+          <t>Bus2_B</t>
+        </is>
+      </c>
+      <c r="L26" s="1" t="inlineStr">
+        <is>
+          <t>Bus2_C</t>
+        </is>
+      </c>
+      <c r="M26" s="1" t="inlineStr">
+        <is>
+          <t>V2 (kV)</t>
+        </is>
+      </c>
+      <c r="N26" s="1" t="inlineStr">
+        <is>
+          <t>S_base2 (kVA)</t>
+        </is>
+      </c>
+      <c r="O26" s="1" t="inlineStr">
+        <is>
+          <t>Conn. type2</t>
+        </is>
+      </c>
+      <c r="P26" s="1" t="inlineStr">
+        <is>
+          <t>Tap 1</t>
+        </is>
+      </c>
+      <c r="Q26" s="1" t="inlineStr">
+        <is>
+          <t>Tap 2</t>
+        </is>
+      </c>
+      <c r="R26" s="1" t="inlineStr">
+        <is>
+          <t>Tap 3</t>
+        </is>
+      </c>
+      <c r="S26" s="1" t="inlineStr">
+        <is>
+          <t>Lowest Tap</t>
+        </is>
+      </c>
+      <c r="T26" s="1" t="inlineStr">
+        <is>
+          <t>Highest Tap</t>
+        </is>
+      </c>
+      <c r="U26" s="1" t="inlineStr">
+        <is>
+          <t>Min Range (%)</t>
+        </is>
+      </c>
+      <c r="V26" s="1" t="inlineStr">
+        <is>
+          <t>Max Range (%)</t>
+        </is>
+      </c>
+      <c r="W26" s="1" t="inlineStr">
+        <is>
+          <t>Z0 leakage (pu)</t>
+        </is>
+      </c>
+      <c r="X26" s="1" t="inlineStr">
+        <is>
+          <t>Z1 leakage (pu)</t>
+        </is>
+      </c>
+      <c r="Y26" s="1" t="inlineStr">
+        <is>
+          <t>X0/R0</t>
+        </is>
+      </c>
+      <c r="Z26" s="1" t="inlineStr">
+        <is>
+          <t>X1/R1</t>
+        </is>
+      </c>
+      <c r="AA26" s="1" t="inlineStr">
+        <is>
+          <t>No Load Loss (kW)</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
         <is>
           <t>End of Multiphase 2W Transformer with Mutual Impedance</t>
         </is>
@@ -4348,7 +4430,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>632_C</t>
+          <t>632_A</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -4363,7 +4445,7 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -4374,7 +4456,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>632_A</t>
+          <t>632_B</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -4389,7 +4471,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -4400,7 +4482,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>632_B</t>
+          <t>632_C</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -4415,7 +4497,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -4426,7 +4508,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>633_C</t>
+          <t>633_A</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -4441,7 +4523,7 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -4452,7 +4534,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>633_A</t>
+          <t>633_B</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -4467,7 +4549,7 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -4478,7 +4560,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>633_B</t>
+          <t>633_C</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -4493,7 +4575,7 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -4504,7 +4586,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>634_C</t>
+          <t>634_A</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -4519,7 +4601,7 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -4530,7 +4612,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>634_A</t>
+          <t>634_B</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -4545,7 +4627,7 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -4556,7 +4638,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>634_B</t>
+          <t>634_C</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -4571,7 +4653,7 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -4582,7 +4664,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>645_C</t>
+          <t>645_B</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -4597,7 +4679,7 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -4608,7 +4690,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>645_B</t>
+          <t>645_C</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -4623,7 +4705,7 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -4634,7 +4716,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>646_C</t>
+          <t>646_B</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -4649,7 +4731,7 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
@@ -4660,7 +4742,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>646_B</t>
+          <t>646_C</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -4675,7 +4757,7 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -4686,7 +4768,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>650_C</t>
+          <t>650_A</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -4701,7 +4783,7 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -4712,7 +4794,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>650_A</t>
+          <t>650_B</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -4727,7 +4809,7 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -4738,7 +4820,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>650_B</t>
+          <t>650_C</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -4753,7 +4835,7 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
@@ -4790,7 +4872,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>670_C</t>
+          <t>670_A</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -4805,7 +4887,7 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -4816,7 +4898,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>670_A</t>
+          <t>670_B</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -4831,7 +4913,7 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
@@ -4842,7 +4924,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>670_B</t>
+          <t>670_C</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -4857,7 +4939,7 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
@@ -4868,7 +4950,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>671_C</t>
+          <t>671_A</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -4883,7 +4965,7 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
@@ -4894,7 +4976,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>671_A</t>
+          <t>671_B</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -4909,7 +4991,7 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
@@ -4920,7 +5002,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>671_B</t>
+          <t>671_C</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -4935,7 +5017,7 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -4946,7 +5028,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>675_C</t>
+          <t>675_A</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -4961,7 +5043,7 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
@@ -4972,7 +5054,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>675_A</t>
+          <t>675_B</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -4987,7 +5069,7 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
@@ -4998,7 +5080,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>675_B</t>
+          <t>675_C</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -5013,7 +5095,7 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
@@ -5024,7 +5106,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>680_C</t>
+          <t>680_A</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -5039,7 +5121,7 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
@@ -5050,7 +5132,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>680_A</t>
+          <t>680_B</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -5065,7 +5147,7 @@
         </is>
       </c>
       <c r="E30" t="n">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
@@ -5076,7 +5158,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>680_B</t>
+          <t>680_C</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -5091,7 +5173,7 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
@@ -5102,7 +5184,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>684_C</t>
+          <t>684_A</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -5117,7 +5199,7 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
@@ -5128,7 +5210,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>684_A</t>
+          <t>684_C</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -5143,7 +5225,7 @@
         </is>
       </c>
       <c r="E33" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
@@ -5154,7 +5236,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>692_C</t>
+          <t>692_A</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -5169,7 +5251,7 @@
         </is>
       </c>
       <c r="E34" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
@@ -5180,7 +5262,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>692_A</t>
+          <t>692_B</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -5195,7 +5277,7 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
@@ -5206,7 +5288,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>692_B</t>
+          <t>692_C</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -5221,7 +5303,7 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
@@ -5232,7 +5314,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>brkr_C</t>
+          <t>brkr_A</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -5247,7 +5329,7 @@
         </is>
       </c>
       <c r="E37" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
@@ -5258,7 +5340,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>brkr_A</t>
+          <t>brkr_B</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -5273,7 +5355,7 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
@@ -5284,7 +5366,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>brkr_B</t>
+          <t>brkr_C</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -5299,7 +5381,7 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
@@ -5362,7 +5444,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>mid_C</t>
+          <t>mid_A</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -5377,7 +5459,7 @@
         </is>
       </c>
       <c r="E42" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
@@ -5388,7 +5470,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>mid_A</t>
+          <t>mid_B</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -5403,7 +5485,7 @@
         </is>
       </c>
       <c r="E43" t="n">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
@@ -5414,7 +5496,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>mid_B</t>
+          <t>mid_C</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -5429,7 +5511,7 @@
         </is>
       </c>
       <c r="E44" t="n">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
@@ -5440,7 +5522,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>rg60_C</t>
+          <t>rg60_A</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -5455,7 +5537,7 @@
         </is>
       </c>
       <c r="E45" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
@@ -5466,7 +5548,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>rg60_A</t>
+          <t>rg60_B</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -5481,7 +5563,7 @@
         </is>
       </c>
       <c r="E46" t="n">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
@@ -5492,7 +5574,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>rg60_B</t>
+          <t>rg60_C</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -5507,7 +5589,7 @@
         </is>
       </c>
       <c r="E47" t="n">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
@@ -5518,7 +5600,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>sourcebus_C</t>
+          <t>sourcebus_A</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -5533,7 +5615,7 @@
         </is>
       </c>
       <c r="E48" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
@@ -5544,7 +5626,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>sourcebus_A</t>
+          <t>sourcebus_B</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -5559,7 +5641,7 @@
         </is>
       </c>
       <c r="E49" t="n">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
@@ -5570,7 +5652,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>sourcebus_B</t>
+          <t>sourcebus_C</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -5585,7 +5667,7 @@
         </is>
       </c>
       <c r="E50" t="n">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
@@ -5622,7 +5704,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>xf1_C</t>
+          <t>xf1_A</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -5637,7 +5719,7 @@
         </is>
       </c>
       <c r="E52" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F52" t="inlineStr">
         <is>
@@ -5648,7 +5730,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>xf1_A</t>
+          <t>xf1_B</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -5663,7 +5745,7 @@
         </is>
       </c>
       <c r="E53" t="n">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F53" t="inlineStr">
         <is>
@@ -5674,7 +5756,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>xf1_B</t>
+          <t>xf1_C</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -5689,7 +5771,7 @@
         </is>
       </c>
       <c r="E54" t="n">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
writing transformer star equivalents, three circuits are converting
</commit_message>
<xml_diff>
--- a/CPYDAR/ieee13x.xlsx
+++ b/CPYDAR/ieee13x.xlsx
@@ -3786,7 +3786,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A11:AA27"/>
+  <dimension ref="A11:AA33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3861,490 +3861,1078 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>sub</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>1</v>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>sourcebus</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>650</t>
-        </is>
-      </c>
-      <c r="E13" t="n">
-        <v>1e-05</v>
-      </c>
-      <c r="F13" t="n">
-        <v>8.000000000000001e-05</v>
-      </c>
-      <c r="G13" t="n">
-        <v>0</v>
-      </c>
-      <c r="H13" t="n">
-        <v>0</v>
-      </c>
-      <c r="I13" t="n">
-        <v>1</v>
-      </c>
-      <c r="J13" t="n">
-        <v>1</v>
-      </c>
-      <c r="K13" t="n">
-        <v>-30</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>xfm1</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>1</v>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>xf1</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>634</t>
-        </is>
-      </c>
-      <c r="E14" t="n">
-        <v>0.011</v>
-      </c>
-      <c r="F14" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="G14" t="n">
-        <v>0</v>
-      </c>
-      <c r="H14" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" t="n">
-        <v>1</v>
-      </c>
-      <c r="J14" t="n">
-        <v>1</v>
-      </c>
-      <c r="K14" t="n">
-        <v>0</v>
+          <t>End of Positive-Sequence 2W Transformer</t>
+        </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>End of Positive-Sequence 2W Transformer</t>
+          <t>Positive-Sequence 3W Transformer</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B16" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="C16" s="1" t="inlineStr">
+        <is>
+          <t>Bus1</t>
+        </is>
+      </c>
+      <c r="D16" s="1" t="inlineStr">
+        <is>
+          <t>Bus2</t>
+        </is>
+      </c>
+      <c r="E16" s="1" t="inlineStr">
+        <is>
+          <t>Bus3</t>
+        </is>
+      </c>
+      <c r="F16" s="1" t="inlineStr">
+        <is>
+          <t>R_12 (pu)</t>
+        </is>
+      </c>
+      <c r="G16" s="1" t="inlineStr">
+        <is>
+          <t>Xl_12 (pu)</t>
+        </is>
+      </c>
+      <c r="H16" s="1" t="inlineStr">
+        <is>
+          <t>R_23 (pu)</t>
+        </is>
+      </c>
+      <c r="I16" s="1" t="inlineStr">
+        <is>
+          <t>Xl_23 (pu)</t>
+        </is>
+      </c>
+      <c r="J16" s="1" t="inlineStr">
+        <is>
+          <t>R_31 (pu)</t>
+        </is>
+      </c>
+      <c r="K16" s="1" t="inlineStr">
+        <is>
+          <t>Xl_31 (pu)</t>
+        </is>
+      </c>
+      <c r="L16" s="1" t="inlineStr">
+        <is>
+          <t>Gmag (pu)</t>
+        </is>
+      </c>
+      <c r="M16" s="1" t="inlineStr">
+        <is>
+          <t>Bmag (pu)</t>
+        </is>
+      </c>
+      <c r="N16" s="1" t="inlineStr">
+        <is>
+          <t>Ratio W1 (pu)</t>
+        </is>
+      </c>
+      <c r="O16" s="1" t="inlineStr">
+        <is>
+          <t>Ratio W2 (pu)</t>
+        </is>
+      </c>
+      <c r="P16" s="1" t="inlineStr">
+        <is>
+          <t>Ratio W3 (pu)</t>
+        </is>
+      </c>
+      <c r="Q16" s="1" t="inlineStr">
+        <is>
+          <t>Phase Shift W1 (deg)</t>
+        </is>
+      </c>
+      <c r="R16" s="1" t="inlineStr">
+        <is>
+          <t>Phase Shift W2 (deg)</t>
+        </is>
+      </c>
+      <c r="S16" s="1" t="inlineStr">
+        <is>
+          <t>Phase Shift W3 (deg)</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Positive-Sequence 3W Transformer</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="1" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="B18" s="1" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
-      </c>
-      <c r="C18" s="1" t="inlineStr">
-        <is>
-          <t>Bus1</t>
-        </is>
-      </c>
-      <c r="D18" s="1" t="inlineStr">
-        <is>
-          <t>Bus2</t>
-        </is>
-      </c>
-      <c r="E18" s="1" t="inlineStr">
-        <is>
-          <t>Bus3</t>
-        </is>
-      </c>
-      <c r="F18" s="1" t="inlineStr">
-        <is>
-          <t>R_12 (pu)</t>
-        </is>
-      </c>
-      <c r="G18" s="1" t="inlineStr">
-        <is>
-          <t>Xl_12 (pu)</t>
-        </is>
-      </c>
-      <c r="H18" s="1" t="inlineStr">
-        <is>
-          <t>R_23 (pu)</t>
-        </is>
-      </c>
-      <c r="I18" s="1" t="inlineStr">
-        <is>
-          <t>Xl_23 (pu)</t>
-        </is>
-      </c>
-      <c r="J18" s="1" t="inlineStr">
-        <is>
-          <t>R_31 (pu)</t>
-        </is>
-      </c>
-      <c r="K18" s="1" t="inlineStr">
-        <is>
-          <t>Xl_31 (pu)</t>
-        </is>
-      </c>
-      <c r="L18" s="1" t="inlineStr">
-        <is>
-          <t>Gmag (pu)</t>
-        </is>
-      </c>
-      <c r="M18" s="1" t="inlineStr">
-        <is>
-          <t>Bmag (pu)</t>
-        </is>
-      </c>
-      <c r="N18" s="1" t="inlineStr">
-        <is>
-          <t>Ratio W1 (pu)</t>
-        </is>
-      </c>
-      <c r="O18" s="1" t="inlineStr">
-        <is>
-          <t>Ratio W2 (pu)</t>
-        </is>
-      </c>
-      <c r="P18" s="1" t="inlineStr">
-        <is>
-          <t>Ratio W3 (pu)</t>
-        </is>
-      </c>
-      <c r="Q18" s="1" t="inlineStr">
-        <is>
-          <t>Phase Shift W1 (deg)</t>
-        </is>
-      </c>
-      <c r="R18" s="1" t="inlineStr">
-        <is>
-          <t>Phase Shift W2 (deg)</t>
-        </is>
-      </c>
-      <c r="S18" s="1" t="inlineStr">
-        <is>
-          <t>Phase Shift W3 (deg)</t>
+          <t>End of Positive-Sequence 3W Transformer</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>End of Positive-Sequence 3W Transformer</t>
+          <t>Multiphase 2W Transformer</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B20" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="C20" s="1" t="inlineStr">
+        <is>
+          <t>Number of phases</t>
+        </is>
+      </c>
+      <c r="D20" s="1" t="inlineStr">
+        <is>
+          <t>Bus1_A</t>
+        </is>
+      </c>
+      <c r="E20" s="1" t="inlineStr">
+        <is>
+          <t>Bus1_B</t>
+        </is>
+      </c>
+      <c r="F20" s="1" t="inlineStr">
+        <is>
+          <t>Bus1_C</t>
+        </is>
+      </c>
+      <c r="G20" s="1" t="inlineStr">
+        <is>
+          <t>V1 (kV)</t>
+        </is>
+      </c>
+      <c r="H20" s="1" t="inlineStr">
+        <is>
+          <t>S_base1 (kVA)</t>
+        </is>
+      </c>
+      <c r="I20" s="1" t="inlineStr">
+        <is>
+          <t>Conn. type1</t>
+        </is>
+      </c>
+      <c r="J20" s="1" t="inlineStr">
+        <is>
+          <t>Bus2_A</t>
+        </is>
+      </c>
+      <c r="K20" s="1" t="inlineStr">
+        <is>
+          <t>Bus2_B</t>
+        </is>
+      </c>
+      <c r="L20" s="1" t="inlineStr">
+        <is>
+          <t>Bus2_C</t>
+        </is>
+      </c>
+      <c r="M20" s="1" t="inlineStr">
+        <is>
+          <t>V2 (kV)</t>
+        </is>
+      </c>
+      <c r="N20" s="1" t="inlineStr">
+        <is>
+          <t>S_base2 (kVA)</t>
+        </is>
+      </c>
+      <c r="O20" s="1" t="inlineStr">
+        <is>
+          <t>Conn. type2</t>
+        </is>
+      </c>
+      <c r="P20" s="1" t="inlineStr">
+        <is>
+          <t>Tap 1</t>
+        </is>
+      </c>
+      <c r="Q20" s="1" t="inlineStr">
+        <is>
+          <t>Tap 2</t>
+        </is>
+      </c>
+      <c r="R20" s="1" t="inlineStr">
+        <is>
+          <t>Tap 3</t>
+        </is>
+      </c>
+      <c r="S20" s="1" t="inlineStr">
+        <is>
+          <t>Lowest Tap</t>
+        </is>
+      </c>
+      <c r="T20" s="1" t="inlineStr">
+        <is>
+          <t>Highest Tap</t>
+        </is>
+      </c>
+      <c r="U20" s="1" t="inlineStr">
+        <is>
+          <t>Min Range (%)</t>
+        </is>
+      </c>
+      <c r="V20" s="1" t="inlineStr">
+        <is>
+          <t>Max Range (%)</t>
+        </is>
+      </c>
+      <c r="W20" s="1" t="inlineStr">
+        <is>
+          <t>X (pu)</t>
+        </is>
+      </c>
+      <c r="X20" s="1" t="inlineStr">
+        <is>
+          <t>RW1 (pu)</t>
+        </is>
+      </c>
+      <c r="Y20" s="1" t="inlineStr">
+        <is>
+          <t>RW2 (pu)</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Multiphase 2W Transformer</t>
-        </is>
+          <t>sub</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" t="n">
+        <v>3</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>sourcebus_A</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>sourcebus_B</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>sourcebus_C</t>
+        </is>
+      </c>
+      <c r="G21" t="n">
+        <v>115</v>
+      </c>
+      <c r="H21" t="n">
+        <v>5000</v>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>delta</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>650_A</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>650_B</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>650_C</t>
+        </is>
+      </c>
+      <c r="M21" t="n">
+        <v>4.16</v>
+      </c>
+      <c r="N21" t="n">
+        <v>5000</v>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>wye</t>
+        </is>
+      </c>
+      <c r="P21" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>0</v>
+      </c>
+      <c r="R21" t="n">
+        <v>0</v>
+      </c>
+      <c r="S21" t="n">
+        <v>-16</v>
+      </c>
+      <c r="T21" t="n">
+        <v>16</v>
+      </c>
+      <c r="U21" t="n">
+        <v>10</v>
+      </c>
+      <c r="V21" t="n">
+        <v>10</v>
+      </c>
+      <c r="W21" t="n">
+        <v>8.000000000000001e-05</v>
+      </c>
+      <c r="X21" t="n">
+        <v>5e-06</v>
+      </c>
+      <c r="Y21" t="n">
+        <v>5e-06</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="1" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="B22" s="1" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
-      </c>
-      <c r="C22" s="1" t="inlineStr">
-        <is>
-          <t>Number of phases</t>
-        </is>
-      </c>
-      <c r="D22" s="1" t="inlineStr">
-        <is>
-          <t>Bus1_A</t>
-        </is>
-      </c>
-      <c r="E22" s="1" t="inlineStr">
-        <is>
-          <t>Bus1_B</t>
-        </is>
-      </c>
-      <c r="F22" s="1" t="inlineStr">
-        <is>
-          <t>Bus1_C</t>
-        </is>
-      </c>
-      <c r="G22" s="1" t="inlineStr">
-        <is>
-          <t>V1 (kV)</t>
-        </is>
-      </c>
-      <c r="H22" s="1" t="inlineStr">
-        <is>
-          <t>S_base1 (kVA)</t>
-        </is>
-      </c>
-      <c r="I22" s="1" t="inlineStr">
-        <is>
-          <t>Conn. type1</t>
-        </is>
-      </c>
-      <c r="J22" s="1" t="inlineStr">
-        <is>
-          <t>Bus2_A</t>
-        </is>
-      </c>
-      <c r="K22" s="1" t="inlineStr">
-        <is>
-          <t>Bus2_B</t>
-        </is>
-      </c>
-      <c r="L22" s="1" t="inlineStr">
-        <is>
-          <t>Bus2_C</t>
-        </is>
-      </c>
-      <c r="M22" s="1" t="inlineStr">
-        <is>
-          <t>V2 (kV)</t>
-        </is>
-      </c>
-      <c r="N22" s="1" t="inlineStr">
-        <is>
-          <t>S_base2 (kVA)</t>
-        </is>
-      </c>
-      <c r="O22" s="1" t="inlineStr">
-        <is>
-          <t>Conn. type2</t>
-        </is>
-      </c>
-      <c r="P22" s="1" t="inlineStr">
-        <is>
-          <t>Tap 1</t>
-        </is>
-      </c>
-      <c r="Q22" s="1" t="inlineStr">
-        <is>
-          <t>Tap 2</t>
-        </is>
-      </c>
-      <c r="R22" s="1" t="inlineStr">
-        <is>
-          <t>Tap 3</t>
-        </is>
-      </c>
-      <c r="S22" s="1" t="inlineStr">
-        <is>
-          <t>Lowest Tap</t>
-        </is>
-      </c>
-      <c r="T22" s="1" t="inlineStr">
-        <is>
-          <t>Highest Tap</t>
-        </is>
-      </c>
-      <c r="U22" s="1" t="inlineStr">
-        <is>
-          <t>Min Range (%)</t>
-        </is>
-      </c>
-      <c r="V22" s="1" t="inlineStr">
-        <is>
-          <t>Max Range (%)</t>
-        </is>
-      </c>
-      <c r="W22" s="1" t="inlineStr">
-        <is>
-          <t>X (pu)</t>
-        </is>
-      </c>
-      <c r="X22" s="1" t="inlineStr">
-        <is>
-          <t>RW1 (pu)</t>
-        </is>
-      </c>
-      <c r="Y22" s="1" t="inlineStr">
-        <is>
-          <t>RW2</t>
-        </is>
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>xfm1</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>1</v>
+      </c>
+      <c r="C22" t="n">
+        <v>3</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>xf1_A</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>xf1_B</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>xf1_C</t>
+        </is>
+      </c>
+      <c r="G22" t="n">
+        <v>4.16</v>
+      </c>
+      <c r="H22" t="n">
+        <v>500</v>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>wye</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>634_A</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>634_B</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>634_C</t>
+        </is>
+      </c>
+      <c r="M22" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="N22" t="n">
+        <v>500</v>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>wye</t>
+        </is>
+      </c>
+      <c r="P22" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>0</v>
+      </c>
+      <c r="R22" t="n">
+        <v>0</v>
+      </c>
+      <c r="S22" t="n">
+        <v>-16</v>
+      </c>
+      <c r="T22" t="n">
+        <v>16</v>
+      </c>
+      <c r="U22" t="n">
+        <v>10</v>
+      </c>
+      <c r="V22" t="n">
+        <v>10</v>
+      </c>
+      <c r="W22" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="X22" t="n">
+        <v>0.005500000000000001</v>
+      </c>
+      <c r="Y22" t="n">
+        <v>0.005500000000000001</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>End of Multiphase 2W Transformer</t>
-        </is>
+          <t>Reg:reg1</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>1</v>
+      </c>
+      <c r="C23" t="n">
+        <v>1</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>brkr_A</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr"/>
+      <c r="G23" t="n">
+        <v>4.156921938165305</v>
+      </c>
+      <c r="H23" t="n">
+        <v>1666</v>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>wye</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>rg60_A</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr"/>
+      <c r="L23" t="inlineStr"/>
+      <c r="M23" t="n">
+        <v>4.156921938165305</v>
+      </c>
+      <c r="N23" t="n">
+        <v>1666</v>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>wye</t>
+        </is>
+      </c>
+      <c r="P23" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>0</v>
+      </c>
+      <c r="R23" t="n">
+        <v>0</v>
+      </c>
+      <c r="S23" t="n">
+        <v>-16</v>
+      </c>
+      <c r="T23" t="n">
+        <v>16</v>
+      </c>
+      <c r="U23" t="n">
+        <v>10</v>
+      </c>
+      <c r="V23" t="n">
+        <v>10</v>
+      </c>
+      <c r="W23" t="n">
+        <v>1.645701472820407e-08</v>
+      </c>
+      <c r="X23" t="n">
+        <v>5e-05</v>
+      </c>
+      <c r="Y23" t="n">
+        <v>5e-05</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Reg:reg2</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>1</v>
+      </c>
+      <c r="C24" t="n">
+        <v>1</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>brkr_B</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="n">
+        <v>4.156921938165305</v>
+      </c>
+      <c r="H24" t="n">
+        <v>1666</v>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>wye</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>rg60_B</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr"/>
+      <c r="L24" t="inlineStr"/>
+      <c r="M24" t="n">
+        <v>4.156921938165305</v>
+      </c>
+      <c r="N24" t="n">
+        <v>1666</v>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>wye</t>
+        </is>
+      </c>
+      <c r="P24" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>0</v>
+      </c>
+      <c r="R24" t="n">
+        <v>0</v>
+      </c>
+      <c r="S24" t="n">
+        <v>-16</v>
+      </c>
+      <c r="T24" t="n">
+        <v>16</v>
+      </c>
+      <c r="U24" t="n">
+        <v>10</v>
+      </c>
+      <c r="V24" t="n">
+        <v>10</v>
+      </c>
+      <c r="W24" t="n">
+        <v>1.645701472820407e-08</v>
+      </c>
+      <c r="X24" t="n">
+        <v>5e-05</v>
+      </c>
+      <c r="Y24" t="n">
+        <v>5e-05</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Multiphase 2W Transformer with Mutual Impedance</t>
-        </is>
+          <t>Reg:reg3</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>1</v>
+      </c>
+      <c r="C25" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>brkr_C</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr"/>
+      <c r="G25" t="n">
+        <v>4.156921938165305</v>
+      </c>
+      <c r="H25" t="n">
+        <v>1666</v>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>wye</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>rg60_C</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr"/>
+      <c r="L25" t="inlineStr"/>
+      <c r="M25" t="n">
+        <v>4.156921938165305</v>
+      </c>
+      <c r="N25" t="n">
+        <v>1666</v>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>wye</t>
+        </is>
+      </c>
+      <c r="P25" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>0</v>
+      </c>
+      <c r="R25" t="n">
+        <v>0</v>
+      </c>
+      <c r="S25" t="n">
+        <v>-16</v>
+      </c>
+      <c r="T25" t="n">
+        <v>16</v>
+      </c>
+      <c r="U25" t="n">
+        <v>10</v>
+      </c>
+      <c r="V25" t="n">
+        <v>10</v>
+      </c>
+      <c r="W25" t="n">
+        <v>1.645701472820407e-08</v>
+      </c>
+      <c r="X25" t="n">
+        <v>5e-05</v>
+      </c>
+      <c r="Y25" t="n">
+        <v>5e-05</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="1" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="B26" s="1" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
-      </c>
-      <c r="C26" s="1" t="inlineStr">
-        <is>
-          <t>Number of phases</t>
-        </is>
-      </c>
-      <c r="D26" s="1" t="inlineStr">
-        <is>
-          <t>Bus1_A</t>
-        </is>
-      </c>
-      <c r="E26" s="1" t="inlineStr">
-        <is>
-          <t>Bus1_B</t>
-        </is>
-      </c>
-      <c r="F26" s="1" t="inlineStr">
-        <is>
-          <t>Bus1_C</t>
-        </is>
-      </c>
-      <c r="G26" s="1" t="inlineStr">
-        <is>
-          <t>V1 (kV)</t>
-        </is>
-      </c>
-      <c r="H26" s="1" t="inlineStr">
-        <is>
-          <t>S_base1 (kVA)</t>
-        </is>
-      </c>
-      <c r="I26" s="1" t="inlineStr">
-        <is>
-          <t>Conn. type1</t>
-        </is>
-      </c>
-      <c r="J26" s="1" t="inlineStr">
-        <is>
-          <t>Bus2_A</t>
-        </is>
-      </c>
-      <c r="K26" s="1" t="inlineStr">
-        <is>
-          <t>Bus2_B</t>
-        </is>
-      </c>
-      <c r="L26" s="1" t="inlineStr">
-        <is>
-          <t>Bus2_C</t>
-        </is>
-      </c>
-      <c r="M26" s="1" t="inlineStr">
-        <is>
-          <t>V2 (kV)</t>
-        </is>
-      </c>
-      <c r="N26" s="1" t="inlineStr">
-        <is>
-          <t>S_base2 (kVA)</t>
-        </is>
-      </c>
-      <c r="O26" s="1" t="inlineStr">
-        <is>
-          <t>Conn. type2</t>
-        </is>
-      </c>
-      <c r="P26" s="1" t="inlineStr">
-        <is>
-          <t>Tap 1</t>
-        </is>
-      </c>
-      <c r="Q26" s="1" t="inlineStr">
-        <is>
-          <t>Tap 2</t>
-        </is>
-      </c>
-      <c r="R26" s="1" t="inlineStr">
-        <is>
-          <t>Tap 3</t>
-        </is>
-      </c>
-      <c r="S26" s="1" t="inlineStr">
-        <is>
-          <t>Lowest Tap</t>
-        </is>
-      </c>
-      <c r="T26" s="1" t="inlineStr">
-        <is>
-          <t>Highest Tap</t>
-        </is>
-      </c>
-      <c r="U26" s="1" t="inlineStr">
-        <is>
-          <t>Min Range (%)</t>
-        </is>
-      </c>
-      <c r="V26" s="1" t="inlineStr">
-        <is>
-          <t>Max Range (%)</t>
-        </is>
-      </c>
-      <c r="W26" s="1" t="inlineStr">
-        <is>
-          <t>Z0 leakage (pu)</t>
-        </is>
-      </c>
-      <c r="X26" s="1" t="inlineStr">
-        <is>
-          <t>Z1 leakage (pu)</t>
-        </is>
-      </c>
-      <c r="Y26" s="1" t="inlineStr">
-        <is>
-          <t>X0/R0</t>
-        </is>
-      </c>
-      <c r="Z26" s="1" t="inlineStr">
-        <is>
-          <t>X1/R1</t>
-        </is>
-      </c>
-      <c r="AA26" s="1" t="inlineStr">
-        <is>
-          <t>No Load Loss (kW)</t>
-        </is>
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>tpoletop:tpoletop</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>1</v>
+      </c>
+      <c r="C26" t="n">
+        <v>1</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>xfstar_tpoletop_B</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="inlineStr"/>
+      <c r="G26" t="n">
+        <v>4.156921938165305</v>
+      </c>
+      <c r="H26" t="n">
+        <v>5</v>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>wye</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>house_s1</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr"/>
+      <c r="L26" t="inlineStr"/>
+      <c r="M26" t="n">
+        <v>0.2078460969082652</v>
+      </c>
+      <c r="N26" t="n">
+        <v>5</v>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>wye</t>
+        </is>
+      </c>
+      <c r="P26" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>0</v>
+      </c>
+      <c r="R26" t="n">
+        <v>0</v>
+      </c>
+      <c r="S26" t="n">
+        <v>-16</v>
+      </c>
+      <c r="T26" t="n">
+        <v>16</v>
+      </c>
+      <c r="U26" t="n">
+        <v>10</v>
+      </c>
+      <c r="V26" t="n">
+        <v>10</v>
+      </c>
+      <c r="W26" t="n">
+        <v>0.001400000000000002</v>
+      </c>
+      <c r="X26" t="n">
+        <v>0.0045</v>
+      </c>
+      <c r="Y26" t="n">
+        <v>0.0045</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
+        <is>
+          <t>tpoletop:tpoletop</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>1</v>
+      </c>
+      <c r="C27" t="n">
+        <v>1</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>xfstar_tpoletop_B</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="inlineStr"/>
+      <c r="G27" t="n">
+        <v>4.156921938165305</v>
+      </c>
+      <c r="H27" t="n">
+        <v>5</v>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>wye</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>house_s2</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr"/>
+      <c r="L27" t="inlineStr"/>
+      <c r="M27" t="n">
+        <v>0.2078460969082652</v>
+      </c>
+      <c r="N27" t="n">
+        <v>5</v>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>wye</t>
+        </is>
+      </c>
+      <c r="P27" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q27" t="n">
+        <v>0</v>
+      </c>
+      <c r="R27" t="n">
+        <v>0</v>
+      </c>
+      <c r="S27" t="n">
+        <v>-16</v>
+      </c>
+      <c r="T27" t="n">
+        <v>16</v>
+      </c>
+      <c r="U27" t="n">
+        <v>10</v>
+      </c>
+      <c r="V27" t="n">
+        <v>10</v>
+      </c>
+      <c r="W27" t="n">
+        <v>0.0122</v>
+      </c>
+      <c r="X27" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y27" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>End of Multiphase 2W Transformer</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Multiphase 2W Transformer with Mutual Impedance</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B31" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="C31" s="1" t="inlineStr">
+        <is>
+          <t>Number of phases</t>
+        </is>
+      </c>
+      <c r="D31" s="1" t="inlineStr">
+        <is>
+          <t>Bus1_A</t>
+        </is>
+      </c>
+      <c r="E31" s="1" t="inlineStr">
+        <is>
+          <t>Bus1_B</t>
+        </is>
+      </c>
+      <c r="F31" s="1" t="inlineStr">
+        <is>
+          <t>Bus1_C</t>
+        </is>
+      </c>
+      <c r="G31" s="1" t="inlineStr">
+        <is>
+          <t>V1 (kV)</t>
+        </is>
+      </c>
+      <c r="H31" s="1" t="inlineStr">
+        <is>
+          <t>S_base1 (kVA)</t>
+        </is>
+      </c>
+      <c r="I31" s="1" t="inlineStr">
+        <is>
+          <t>Conn. type1</t>
+        </is>
+      </c>
+      <c r="J31" s="1" t="inlineStr">
+        <is>
+          <t>Bus2_A</t>
+        </is>
+      </c>
+      <c r="K31" s="1" t="inlineStr">
+        <is>
+          <t>Bus2_B</t>
+        </is>
+      </c>
+      <c r="L31" s="1" t="inlineStr">
+        <is>
+          <t>Bus2_C</t>
+        </is>
+      </c>
+      <c r="M31" s="1" t="inlineStr">
+        <is>
+          <t>V2 (kV)</t>
+        </is>
+      </c>
+      <c r="N31" s="1" t="inlineStr">
+        <is>
+          <t>S_base2 (kVA)</t>
+        </is>
+      </c>
+      <c r="O31" s="1" t="inlineStr">
+        <is>
+          <t>Conn. type2</t>
+        </is>
+      </c>
+      <c r="P31" s="1" t="inlineStr">
+        <is>
+          <t>Tap 1</t>
+        </is>
+      </c>
+      <c r="Q31" s="1" t="inlineStr">
+        <is>
+          <t>Tap 2</t>
+        </is>
+      </c>
+      <c r="R31" s="1" t="inlineStr">
+        <is>
+          <t>Tap 3</t>
+        </is>
+      </c>
+      <c r="S31" s="1" t="inlineStr">
+        <is>
+          <t>Lowest Tap</t>
+        </is>
+      </c>
+      <c r="T31" s="1" t="inlineStr">
+        <is>
+          <t>Highest Tap</t>
+        </is>
+      </c>
+      <c r="U31" s="1" t="inlineStr">
+        <is>
+          <t>Min Range (%)</t>
+        </is>
+      </c>
+      <c r="V31" s="1" t="inlineStr">
+        <is>
+          <t>Max Range (%)</t>
+        </is>
+      </c>
+      <c r="W31" s="1" t="inlineStr">
+        <is>
+          <t>Z0 leakage (pu)</t>
+        </is>
+      </c>
+      <c r="X31" s="1" t="inlineStr">
+        <is>
+          <t>Z1 leakage (pu)</t>
+        </is>
+      </c>
+      <c r="Y31" s="1" t="inlineStr">
+        <is>
+          <t>X0/R0</t>
+        </is>
+      </c>
+      <c r="Z31" s="1" t="inlineStr">
+        <is>
+          <t>X1/R1</t>
+        </is>
+      </c>
+      <c r="AA31" s="1" t="inlineStr">
+        <is>
+          <t>No Load Loss (kW)</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>tpoletop:tpoletop</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>1</v>
+      </c>
+      <c r="C32" t="n">
+        <v>1</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>670_B</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr"/>
+      <c r="F32" t="inlineStr"/>
+      <c r="G32" t="n">
+        <v>4.156921938165305</v>
+      </c>
+      <c r="H32" t="n">
+        <v>5</v>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>wye</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>xfstar_tpoletop_B</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr"/>
+      <c r="L32" t="inlineStr"/>
+      <c r="M32" t="n">
+        <v>4.156921938165305</v>
+      </c>
+      <c r="N32" t="n">
+        <v>5</v>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>wye</t>
+        </is>
+      </c>
+      <c r="P32" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>0</v>
+      </c>
+      <c r="R32" t="n">
+        <v>0</v>
+      </c>
+      <c r="S32" t="n">
+        <v>-16</v>
+      </c>
+      <c r="T32" t="n">
+        <v>16</v>
+      </c>
+      <c r="U32" t="n">
+        <v>10</v>
+      </c>
+      <c r="V32" t="n">
+        <v>10</v>
+      </c>
+      <c r="W32" t="n">
+        <v>0.01217538500417954</v>
+      </c>
+      <c r="X32" t="n">
+        <v>0.01217538500417954</v>
+      </c>
+      <c r="Y32" t="n">
+        <v>0.9111111111111114</v>
+      </c>
+      <c r="Z32" t="n">
+        <v>0.9111111111111114</v>
+      </c>
+      <c r="AA32" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
         <is>
           <t>End of Multiphase 2W Transformer with Mutual Impedance</t>
         </is>
@@ -4361,7 +4949,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F54"/>
+  <dimension ref="A1:F55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5392,7 +5980,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>house_s2</t>
+          <t>house_s1</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -5407,7 +5995,7 @@
         </is>
       </c>
       <c r="E40" t="n">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
@@ -5418,7 +6006,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>house_s1</t>
+          <t>house_s2</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -5433,7 +6021,7 @@
         </is>
       </c>
       <c r="E41" t="n">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
@@ -5774,6 +6362,32 @@
         <v>120</v>
       </c>
       <c r="F54" t="inlineStr">
+        <is>
+          <t>PQ</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>xfstar_tpoletop_B</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>2400</v>
+      </c>
+      <c r="C55" t="n">
+        <v>1</v>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>pu</t>
+        </is>
+      </c>
+      <c r="E55" t="n">
+        <v>-120</v>
+      </c>
+      <c r="F55" t="inlineStr">
         <is>
           <t>PQ</t>
         </is>

</xml_diff>

<commit_message>
fixed ShortCircuitTest conversion for 3-winding transformers
</commit_message>
<xml_diff>
--- a/CPYDAR/ieee13x.xlsx
+++ b/CPYDAR/ieee13x.xlsx
@@ -4370,13 +4370,13 @@
         <v>10</v>
       </c>
       <c r="W23" t="n">
-        <v>1.645701472820407e-08</v>
+        <v>0.0001000000013541667</v>
       </c>
       <c r="X23" t="n">
-        <v>5e-05</v>
+        <v>5.000000067708333e-05</v>
       </c>
       <c r="Y23" t="n">
-        <v>5e-05</v>
+        <v>5.000000067708333e-05</v>
       </c>
     </row>
     <row r="24">
@@ -4449,13 +4449,13 @@
         <v>10</v>
       </c>
       <c r="W24" t="n">
-        <v>1.645701472820407e-08</v>
+        <v>0.0001000000013541667</v>
       </c>
       <c r="X24" t="n">
-        <v>5e-05</v>
+        <v>5.000000067708333e-05</v>
       </c>
       <c r="Y24" t="n">
-        <v>5e-05</v>
+        <v>5.000000067708333e-05</v>
       </c>
     </row>
     <row r="25">
@@ -4528,13 +4528,13 @@
         <v>10</v>
       </c>
       <c r="W25" t="n">
-        <v>1.645701472820407e-08</v>
+        <v>0.0001000000013541667</v>
       </c>
       <c r="X25" t="n">
-        <v>5e-05</v>
+        <v>5.000000067708333e-05</v>
       </c>
       <c r="Y25" t="n">
-        <v>5e-05</v>
+        <v>5.000000067708333e-05</v>
       </c>
     </row>
     <row r="26">
@@ -4551,7 +4551,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>xfstar_tpoletop_B</t>
+          <t>xfbus_tpoletop_B</t>
         </is>
       </c>
       <c r="E26" t="inlineStr"/>
@@ -4607,13 +4607,13 @@
         <v>10</v>
       </c>
       <c r="W26" t="n">
-        <v>0.001400000000000002</v>
+        <v>0.0068</v>
       </c>
       <c r="X26" t="n">
-        <v>0.0045</v>
+        <v>0.006</v>
       </c>
       <c r="Y26" t="n">
-        <v>0.0045</v>
+        <v>0.006</v>
       </c>
     </row>
     <row r="27">
@@ -4630,7 +4630,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>xfstar_tpoletop_B</t>
+          <t>xfbus_tpoletop_B</t>
         </is>
       </c>
       <c r="E27" t="inlineStr"/>
@@ -4686,13 +4686,13 @@
         <v>10</v>
       </c>
       <c r="W27" t="n">
-        <v>0.0122</v>
+        <v>0.0068</v>
       </c>
       <c r="X27" t="n">
-        <v>0</v>
+        <v>0.006</v>
       </c>
       <c r="Y27" t="n">
-        <v>0</v>
+        <v>0.006</v>
       </c>
     </row>
     <row r="28">
@@ -4878,7 +4878,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>xfstar_tpoletop_B</t>
+          <t>xfbus_tpoletop_B</t>
         </is>
       </c>
       <c r="K32" t="inlineStr"/>
@@ -4916,16 +4916,16 @@
         <v>10</v>
       </c>
       <c r="W32" t="n">
-        <v>0.01217538500417954</v>
+        <v>0.01486472334084964</v>
       </c>
       <c r="X32" t="n">
-        <v>0.01217538500417954</v>
+        <v>0.01486472334084964</v>
       </c>
       <c r="Y32" t="n">
-        <v>0.9111111111111114</v>
+        <v>2.266666666666666</v>
       </c>
       <c r="Z32" t="n">
-        <v>0.9111111111111114</v>
+        <v>2.266666666666666</v>
       </c>
       <c r="AA32" t="n">
         <v>0.01</v>
@@ -5018,7 +5018,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>632_A</t>
+          <t>632_C</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -5033,7 +5033,7 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -5044,7 +5044,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>632_B</t>
+          <t>632_A</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -5059,7 +5059,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -5070,7 +5070,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>632_C</t>
+          <t>632_B</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -5085,7 +5085,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -5096,7 +5096,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>633_A</t>
+          <t>633_C</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -5111,7 +5111,7 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -5122,7 +5122,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>633_B</t>
+          <t>633_A</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -5137,7 +5137,7 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -5148,7 +5148,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>633_C</t>
+          <t>633_B</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -5163,7 +5163,7 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -5174,7 +5174,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>634_A</t>
+          <t>634_C</t>
         </is>
       </c>
       <c r="B9" t="n">
@@ -5189,7 +5189,7 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -5200,7 +5200,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>634_B</t>
+          <t>634_A</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -5215,7 +5215,7 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -5226,7 +5226,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>634_C</t>
+          <t>634_B</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -5241,7 +5241,7 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -5252,7 +5252,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>645_B</t>
+          <t>645_C</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -5267,7 +5267,7 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -5278,7 +5278,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>645_C</t>
+          <t>645_B</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -5293,7 +5293,7 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -5304,7 +5304,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>646_B</t>
+          <t>646_C</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -5319,7 +5319,7 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>-120</v>
+        <v>120</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
@@ -5330,7 +5330,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>646_C</t>
+          <t>646_B</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -5345,7 +5345,7 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -5356,7 +5356,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>650_A</t>
+          <t>650_C</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -5371,7 +5371,7 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -5382,7 +5382,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>650_B</t>
+          <t>650_A</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -5397,7 +5397,7 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -5408,7 +5408,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>650_C</t>
+          <t>650_B</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -5423,7 +5423,7 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
@@ -5460,7 +5460,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>670_A</t>
+          <t>670_C</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -5475,7 +5475,7 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -5486,7 +5486,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>670_B</t>
+          <t>670_A</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -5501,7 +5501,7 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
@@ -5512,7 +5512,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>670_C</t>
+          <t>670_B</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -5527,7 +5527,7 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
@@ -5538,7 +5538,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>671_A</t>
+          <t>671_C</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -5553,7 +5553,7 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
@@ -5564,7 +5564,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>671_B</t>
+          <t>671_A</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -5579,7 +5579,7 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
@@ -5590,7 +5590,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>671_C</t>
+          <t>671_B</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -5605,7 +5605,7 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -5616,7 +5616,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>675_A</t>
+          <t>675_C</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -5631,7 +5631,7 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
@@ -5642,7 +5642,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>675_B</t>
+          <t>675_A</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -5657,7 +5657,7 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
@@ -5668,7 +5668,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>675_C</t>
+          <t>675_B</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -5683,7 +5683,7 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
@@ -5694,7 +5694,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>680_A</t>
+          <t>680_C</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -5709,7 +5709,7 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
@@ -5720,7 +5720,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>680_B</t>
+          <t>680_A</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -5735,7 +5735,7 @@
         </is>
       </c>
       <c r="E30" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
@@ -5746,7 +5746,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>680_C</t>
+          <t>680_B</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -5761,7 +5761,7 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
@@ -5772,7 +5772,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>684_A</t>
+          <t>684_C</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -5787,7 +5787,7 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
@@ -5798,7 +5798,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>684_C</t>
+          <t>684_A</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -5813,7 +5813,7 @@
         </is>
       </c>
       <c r="E33" t="n">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
@@ -5824,7 +5824,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>692_A</t>
+          <t>692_C</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -5839,7 +5839,7 @@
         </is>
       </c>
       <c r="E34" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
@@ -5850,7 +5850,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>692_B</t>
+          <t>692_A</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -5865,7 +5865,7 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
@@ -5876,7 +5876,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>692_C</t>
+          <t>692_B</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -5891,7 +5891,7 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
@@ -5902,7 +5902,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>brkr_A</t>
+          <t>brkr_C</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -5917,7 +5917,7 @@
         </is>
       </c>
       <c r="E37" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
@@ -5928,7 +5928,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>brkr_B</t>
+          <t>brkr_A</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -5943,7 +5943,7 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
@@ -5954,7 +5954,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>brkr_C</t>
+          <t>brkr_B</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -5969,7 +5969,7 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
@@ -6032,7 +6032,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>mid_A</t>
+          <t>mid_C</t>
         </is>
       </c>
       <c r="B42" t="n">
@@ -6047,7 +6047,7 @@
         </is>
       </c>
       <c r="E42" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
@@ -6058,7 +6058,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>mid_B</t>
+          <t>mid_A</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -6073,7 +6073,7 @@
         </is>
       </c>
       <c r="E43" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
@@ -6084,7 +6084,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>mid_C</t>
+          <t>mid_B</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -6099,7 +6099,7 @@
         </is>
       </c>
       <c r="E44" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
@@ -6110,7 +6110,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>rg60_A</t>
+          <t>rg60_C</t>
         </is>
       </c>
       <c r="B45" t="n">
@@ -6125,7 +6125,7 @@
         </is>
       </c>
       <c r="E45" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
@@ -6136,7 +6136,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>rg60_B</t>
+          <t>rg60_A</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -6151,7 +6151,7 @@
         </is>
       </c>
       <c r="E46" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
@@ -6162,7 +6162,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>rg60_C</t>
+          <t>rg60_B</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -6177,7 +6177,7 @@
         </is>
       </c>
       <c r="E47" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
@@ -6188,7 +6188,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>sourcebus_A</t>
+          <t>sourcebus_C</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -6203,7 +6203,7 @@
         </is>
       </c>
       <c r="E48" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
@@ -6214,7 +6214,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>sourcebus_B</t>
+          <t>sourcebus_A</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -6229,7 +6229,7 @@
         </is>
       </c>
       <c r="E49" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
@@ -6240,7 +6240,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>sourcebus_C</t>
+          <t>sourcebus_B</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -6255,7 +6255,7 @@
         </is>
       </c>
       <c r="E50" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
@@ -6292,7 +6292,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>xf1_A</t>
+          <t>xf1_C</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -6307,7 +6307,7 @@
         </is>
       </c>
       <c r="E52" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F52" t="inlineStr">
         <is>
@@ -6318,7 +6318,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>xf1_B</t>
+          <t>xf1_A</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -6333,7 +6333,7 @@
         </is>
       </c>
       <c r="E53" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F53" t="inlineStr">
         <is>
@@ -6344,7 +6344,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>xf1_C</t>
+          <t>xf1_B</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -6359,7 +6359,7 @@
         </is>
       </c>
       <c r="E54" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>
@@ -6370,7 +6370,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>xfstar_tpoletop_B</t>
+          <t>xfbus_tpoletop_B</t>
         </is>
       </c>
       <c r="B55" t="n">

</xml_diff>

<commit_message>
capitalizing global constants, locking default taps to 0 with no range
</commit_message>
<xml_diff>
--- a/CPYDAR/ieee13x.xlsx
+++ b/CPYDAR/ieee13x.xlsx
@@ -4184,16 +4184,16 @@
         <v>0</v>
       </c>
       <c r="S21" t="n">
-        <v>-16</v>
+        <v>0</v>
       </c>
       <c r="T21" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="U21" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="V21" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="W21" t="n">
         <v>8.000000000000001e-05</v>
@@ -4279,16 +4279,16 @@
         <v>0</v>
       </c>
       <c r="S22" t="n">
-        <v>-16</v>
+        <v>0</v>
       </c>
       <c r="T22" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="U22" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="V22" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="W22" t="n">
         <v>0.02</v>
@@ -4358,16 +4358,16 @@
         <v>0</v>
       </c>
       <c r="S23" t="n">
-        <v>-16</v>
+        <v>0</v>
       </c>
       <c r="T23" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="U23" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="V23" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="W23" t="n">
         <v>0.0001000000013541667</v>
@@ -4437,16 +4437,16 @@
         <v>0</v>
       </c>
       <c r="S24" t="n">
-        <v>-16</v>
+        <v>0</v>
       </c>
       <c r="T24" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="U24" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="V24" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="W24" t="n">
         <v>0.0001000000013541667</v>
@@ -4516,16 +4516,16 @@
         <v>0</v>
       </c>
       <c r="S25" t="n">
-        <v>-16</v>
+        <v>0</v>
       </c>
       <c r="T25" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="U25" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="V25" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="W25" t="n">
         <v>0.0001000000013541667</v>
@@ -4595,16 +4595,16 @@
         <v>0</v>
       </c>
       <c r="S26" t="n">
-        <v>-16</v>
+        <v>0</v>
       </c>
       <c r="T26" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="U26" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="V26" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="W26" t="n">
         <v>0.0068</v>
@@ -4674,16 +4674,16 @@
         <v>0</v>
       </c>
       <c r="S27" t="n">
-        <v>-16</v>
+        <v>0</v>
       </c>
       <c r="T27" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="U27" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="V27" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="W27" t="n">
         <v>0.0068</v>
@@ -4904,16 +4904,16 @@
         <v>0</v>
       </c>
       <c r="S32" t="n">
-        <v>-16</v>
+        <v>0</v>
       </c>
       <c r="T32" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="U32" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="V32" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="W32" t="n">
         <v>0.01486472334084964</v>
@@ -5980,7 +5980,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>house_s1</t>
+          <t>house_s2</t>
         </is>
       </c>
       <c r="B40" t="n">
@@ -5995,7 +5995,7 @@
         </is>
       </c>
       <c r="E40" t="n">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
@@ -6006,7 +6006,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>house_s2</t>
+          <t>house_s1</t>
         </is>
       </c>
       <c r="B41" t="n">
@@ -6021,7 +6021,7 @@
         </is>
       </c>
       <c r="E41" t="n">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
setting taps from banked or tanked regulators
</commit_message>
<xml_diff>
--- a/CPYDAR/ieee13x.xlsx
+++ b/CPYDAR/ieee13x.xlsx
@@ -4349,7 +4349,7 @@
         </is>
       </c>
       <c r="P23" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Q23" t="n">
         <v>0</v>
@@ -4358,16 +4358,16 @@
         <v>0</v>
       </c>
       <c r="S23" t="n">
-        <v>0</v>
+        <v>-16</v>
       </c>
       <c r="T23" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="U23" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="V23" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="W23" t="n">
         <v>0.0001000000013541667</v>
@@ -4428,7 +4428,7 @@
         </is>
       </c>
       <c r="P24" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Q24" t="n">
         <v>0</v>
@@ -4437,16 +4437,16 @@
         <v>0</v>
       </c>
       <c r="S24" t="n">
-        <v>0</v>
+        <v>-16</v>
       </c>
       <c r="T24" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="U24" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="V24" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="W24" t="n">
         <v>0.0001000000013541667</v>
@@ -4507,7 +4507,7 @@
         </is>
       </c>
       <c r="P25" t="n">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="Q25" t="n">
         <v>0</v>
@@ -4516,16 +4516,16 @@
         <v>0</v>
       </c>
       <c r="S25" t="n">
-        <v>0</v>
+        <v>-16</v>
       </c>
       <c r="T25" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="U25" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="V25" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="W25" t="n">
         <v>0.0001000000013541667</v>
@@ -5044,7 +5044,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>632_A</t>
+          <t>632_B</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -5059,7 +5059,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -5070,7 +5070,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>632_B</t>
+          <t>632_A</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -5085,7 +5085,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -5122,7 +5122,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>633_A</t>
+          <t>633_B</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -5137,7 +5137,7 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -5148,7 +5148,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>633_B</t>
+          <t>633_A</t>
         </is>
       </c>
       <c r="B8" t="n">
@@ -5163,7 +5163,7 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -5200,7 +5200,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>634_A</t>
+          <t>634_B</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -5215,7 +5215,7 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -5226,7 +5226,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>634_B</t>
+          <t>634_A</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -5241,7 +5241,7 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -5382,7 +5382,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>650_A</t>
+          <t>650_B</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -5397,7 +5397,7 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -5408,7 +5408,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>650_B</t>
+          <t>650_A</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -5423,7 +5423,7 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
@@ -5486,7 +5486,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>670_A</t>
+          <t>670_B</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -5501,7 +5501,7 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
@@ -5512,7 +5512,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>670_B</t>
+          <t>670_A</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -5527,7 +5527,7 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
@@ -5564,7 +5564,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>671_A</t>
+          <t>671_B</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -5579,7 +5579,7 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
@@ -5590,7 +5590,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>671_B</t>
+          <t>671_A</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -5605,7 +5605,7 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -5642,7 +5642,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>675_A</t>
+          <t>675_B</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -5657,7 +5657,7 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
@@ -5668,7 +5668,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>675_B</t>
+          <t>675_A</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -5683,7 +5683,7 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
@@ -5720,7 +5720,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>680_A</t>
+          <t>680_B</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -5735,7 +5735,7 @@
         </is>
       </c>
       <c r="E30" t="n">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
@@ -5746,7 +5746,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>680_B</t>
+          <t>680_A</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -5761,7 +5761,7 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
@@ -5824,7 +5824,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>692_C</t>
+          <t>692_B</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -5839,7 +5839,7 @@
         </is>
       </c>
       <c r="E34" t="n">
-        <v>120</v>
+        <v>-120</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
@@ -5850,7 +5850,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>692_A</t>
+          <t>692_C</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -5865,7 +5865,7 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
@@ -5876,7 +5876,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>692_B</t>
+          <t>692_A</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -5891,7 +5891,7 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
@@ -5928,7 +5928,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>brkr_A</t>
+          <t>brkr_B</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -5943,7 +5943,7 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
@@ -5954,7 +5954,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>brkr_B</t>
+          <t>brkr_A</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -5969,7 +5969,7 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
@@ -6058,7 +6058,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>mid_A</t>
+          <t>mid_B</t>
         </is>
       </c>
       <c r="B43" t="n">
@@ -6073,7 +6073,7 @@
         </is>
       </c>
       <c r="E43" t="n">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
@@ -6084,7 +6084,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>mid_B</t>
+          <t>mid_A</t>
         </is>
       </c>
       <c r="B44" t="n">
@@ -6099,7 +6099,7 @@
         </is>
       </c>
       <c r="E44" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
@@ -6136,7 +6136,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>rg60_A</t>
+          <t>rg60_B</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -6151,7 +6151,7 @@
         </is>
       </c>
       <c r="E46" t="n">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
@@ -6162,7 +6162,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>rg60_B</t>
+          <t>rg60_A</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -6177,7 +6177,7 @@
         </is>
       </c>
       <c r="E47" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
@@ -6214,7 +6214,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>sourcebus_A</t>
+          <t>sourcebus_B</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -6229,7 +6229,7 @@
         </is>
       </c>
       <c r="E49" t="n">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
@@ -6240,7 +6240,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>sourcebus_B</t>
+          <t>sourcebus_A</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -6255,7 +6255,7 @@
         </is>
       </c>
       <c r="E50" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
@@ -6318,7 +6318,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>xf1_A</t>
+          <t>xf1_B</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -6333,7 +6333,7 @@
         </is>
       </c>
       <c r="E53" t="n">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="F53" t="inlineStr">
         <is>
@@ -6344,7 +6344,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>xf1_B</t>
+          <t>xf1_A</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -6359,7 +6359,7 @@
         </is>
       </c>
       <c r="E54" t="n">
-        <v>-120</v>
+        <v>0</v>
       </c>
       <c r="F54" t="inlineStr">
         <is>

</xml_diff>